<commit_message>
Update DS_LOP_(Mau).xlsx to reflect recent data changes
</commit_message>
<xml_diff>
--- a/data_base/DS_LOP_(Mau).xlsx
+++ b/data_base/DS_LOP_(Mau).xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sumik\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sumik\Downloads\ke-khai-gio-day-app-master\data_base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{725F3DCE-1E63-4273-A819-1E64C8E0E023}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EFC94E4-D914-4F07-B8E8-AA3304244327}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9BE4D872-0846-4818-A986-007578B8C884}"/>
   </bookViews>
@@ -5720,7 +5720,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -5958,31 +5958,19 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -5997,17 +5985,26 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -6384,8 +6381,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:L122"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A88" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I110" sqref="I110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -6419,7 +6416,7 @@
       <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="103"/>
+      <c r="F1" s="89"/>
       <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
@@ -6455,7 +6452,7 @@
         <f t="shared" ref="E2:E63" si="0">INDEX(L:L,MATCH(IF(MID(B2,3,1)="T","TC_"&amp;C2,"CĐ_"&amp;C2),J:J,0),1)</f>
         <v>214</v>
       </c>
-      <c r="F2" s="100"/>
+      <c r="F2" s="87"/>
       <c r="G2" s="9">
         <v>6510216</v>
       </c>
@@ -6488,14 +6485,14 @@
         <v>14</v>
       </c>
       <c r="D3" s="7" t="str">
-        <f t="shared" ref="D2:D65" si="1">UPPER(INDEX(I:I,MATCH(C3,H:H,0),1))</f>
+        <f t="shared" ref="D3:D65" si="1">UPPER(INDEX(I:I,MATCH(C3,H:H,0),1))</f>
         <v>CHẾ BIẾN MÓN ĂN</v>
       </c>
       <c r="E3" s="8" t="str">
         <f t="shared" si="0"/>
         <v>213</v>
       </c>
-      <c r="F3" s="100"/>
+      <c r="F3" s="87"/>
       <c r="G3" s="9">
         <v>6510202</v>
       </c>
@@ -6535,7 +6532,7 @@
         <f t="shared" si="0"/>
         <v>203</v>
       </c>
-      <c r="F4" s="100"/>
+      <c r="F4" s="87"/>
       <c r="G4" s="9">
         <v>6510303</v>
       </c>
@@ -6575,7 +6572,7 @@
         <f t="shared" si="0"/>
         <v>201</v>
       </c>
-      <c r="F5" s="100"/>
+      <c r="F5" s="87"/>
       <c r="G5" s="9">
         <v>6520227</v>
       </c>
@@ -6612,7 +6609,7 @@
         <f t="shared" si="0"/>
         <v>201</v>
       </c>
-      <c r="F6" s="100"/>
+      <c r="F6" s="87"/>
       <c r="G6" s="9">
         <v>6520201</v>
       </c>
@@ -6647,7 +6644,7 @@
         <f t="shared" si="0"/>
         <v>201</v>
       </c>
-      <c r="F7" s="100"/>
+      <c r="F7" s="87"/>
       <c r="G7" s="9">
         <v>6520205</v>
       </c>
@@ -6684,7 +6681,7 @@
         <f t="shared" si="0"/>
         <v>201</v>
       </c>
-      <c r="F8" s="100"/>
+      <c r="F8" s="87"/>
       <c r="G8" s="9">
         <v>6480201</v>
       </c>
@@ -6721,7 +6718,7 @@
         <f t="shared" si="0"/>
         <v>201</v>
       </c>
-      <c r="F9" s="100"/>
+      <c r="F9" s="87"/>
       <c r="G9" s="9">
         <v>6480202</v>
       </c>
@@ -6756,7 +6753,7 @@
         <f t="shared" si="0"/>
         <v>204</v>
       </c>
-      <c r="F10" s="100"/>
+      <c r="F10" s="87"/>
       <c r="G10" s="9">
         <v>6340302</v>
       </c>
@@ -6791,7 +6788,7 @@
         <f t="shared" si="0"/>
         <v>204</v>
       </c>
-      <c r="F11" s="100"/>
+      <c r="F11" s="87"/>
       <c r="G11" s="9">
         <v>6520121</v>
       </c>
@@ -6828,7 +6825,7 @@
         <f t="shared" si="0"/>
         <v>204</v>
       </c>
-      <c r="F12" s="100"/>
+      <c r="F12" s="87"/>
       <c r="G12" s="9">
         <v>6520123</v>
       </c>
@@ -6865,7 +6862,7 @@
         <f t="shared" si="0"/>
         <v>222</v>
       </c>
-      <c r="F13" s="100"/>
+      <c r="F13" s="87"/>
       <c r="G13" s="9">
         <v>6580201</v>
       </c>
@@ -6900,7 +6897,7 @@
         <f t="shared" si="0"/>
         <v>215</v>
       </c>
-      <c r="F14" s="100"/>
+      <c r="F14" s="87"/>
       <c r="G14" s="9">
         <v>6540205</v>
       </c>
@@ -6935,7 +6932,7 @@
         <f t="shared" si="0"/>
         <v>216</v>
       </c>
-      <c r="F15" s="100"/>
+      <c r="F15" s="87"/>
       <c r="G15" s="9">
         <v>6320301</v>
       </c>
@@ -6970,7 +6967,7 @@
         <f t="shared" si="0"/>
         <v>223</v>
       </c>
-      <c r="F16" s="100"/>
+      <c r="F16" s="87"/>
       <c r="G16" s="9">
         <v>6810207</v>
       </c>
@@ -7005,7 +7002,7 @@
         <f t="shared" si="0"/>
         <v>209</v>
       </c>
-      <c r="F17" s="100"/>
+      <c r="F17" s="87"/>
       <c r="G17" s="9">
         <v>6640101</v>
       </c>
@@ -7042,7 +7039,7 @@
         <f t="shared" si="0"/>
         <v>209</v>
       </c>
-      <c r="F18" s="100"/>
+      <c r="F18" s="87"/>
       <c r="G18" s="9">
         <v>6620116</v>
       </c>
@@ -7079,7 +7076,7 @@
         <f t="shared" si="0"/>
         <v>205</v>
       </c>
-      <c r="F19" s="100"/>
+      <c r="F19" s="87"/>
       <c r="G19" s="9">
         <v>6620117</v>
       </c>
@@ -7116,7 +7113,7 @@
         <f t="shared" si="0"/>
         <v>207</v>
       </c>
-      <c r="F20" s="100"/>
+      <c r="F20" s="87"/>
       <c r="G20" s="15">
         <v>5510216</v>
       </c>
@@ -7153,7 +7150,7 @@
         <f t="shared" si="0"/>
         <v>217</v>
       </c>
-      <c r="F21" s="100"/>
+      <c r="F21" s="87"/>
       <c r="G21" s="15">
         <v>5520227</v>
       </c>
@@ -7190,7 +7187,7 @@
         <f t="shared" si="0"/>
         <v>220</v>
       </c>
-      <c r="F22" s="100"/>
+      <c r="F22" s="87"/>
       <c r="G22" s="15">
         <v>5520201</v>
       </c>
@@ -7227,7 +7224,7 @@
         <f t="shared" si="0"/>
         <v>221</v>
       </c>
-      <c r="F23" s="100"/>
+      <c r="F23" s="87"/>
       <c r="G23" s="15">
         <v>5520205</v>
       </c>
@@ -7264,7 +7261,7 @@
         <f t="shared" si="0"/>
         <v>221</v>
       </c>
-      <c r="F24" s="100"/>
+      <c r="F24" s="87"/>
       <c r="G24" s="15">
         <v>5520225</v>
       </c>
@@ -7301,7 +7298,7 @@
         <f t="shared" si="0"/>
         <v>208</v>
       </c>
-      <c r="F25" s="100"/>
+      <c r="F25" s="87"/>
       <c r="G25" s="15">
         <v>5480105</v>
       </c>
@@ -7338,7 +7335,7 @@
         <f t="shared" si="0"/>
         <v>218</v>
       </c>
-      <c r="F26" s="100"/>
+      <c r="F26" s="87"/>
       <c r="G26" s="15">
         <v>5480202</v>
       </c>
@@ -7375,7 +7372,7 @@
         <f t="shared" si="0"/>
         <v>219</v>
       </c>
-      <c r="F27" s="100"/>
+      <c r="F27" s="87"/>
       <c r="G27" s="15">
         <v>5340302</v>
       </c>
@@ -7412,7 +7409,7 @@
         <f t="shared" si="0"/>
         <v>101</v>
       </c>
-      <c r="F28" s="100"/>
+      <c r="F28" s="87"/>
       <c r="G28" s="15">
         <v>5520121</v>
       </c>
@@ -7449,7 +7446,7 @@
         <f t="shared" si="0"/>
         <v>101</v>
       </c>
-      <c r="F29" s="100"/>
+      <c r="F29" s="87"/>
       <c r="G29" s="15">
         <v>5520123</v>
       </c>
@@ -7486,7 +7483,7 @@
         <f t="shared" si="0"/>
         <v>102</v>
       </c>
-      <c r="F30" s="100"/>
+      <c r="F30" s="87"/>
       <c r="G30" s="15">
         <v>5510217</v>
       </c>
@@ -7523,7 +7520,7 @@
         <f t="shared" si="0"/>
         <v>102</v>
       </c>
-      <c r="F31" s="100"/>
+      <c r="F31" s="87"/>
       <c r="G31" s="15">
         <v>5580201</v>
       </c>
@@ -7560,7 +7557,7 @@
         <f t="shared" si="0"/>
         <v>103</v>
       </c>
-      <c r="F32" s="100"/>
+      <c r="F32" s="87"/>
       <c r="G32" s="15">
         <v>5210422</v>
       </c>
@@ -7597,7 +7594,7 @@
         <f t="shared" si="0"/>
         <v>106</v>
       </c>
-      <c r="F33" s="100"/>
+      <c r="F33" s="87"/>
       <c r="G33" s="15">
         <v>5540205</v>
       </c>
@@ -7634,7 +7631,7 @@
         <f t="shared" si="0"/>
         <v>111</v>
       </c>
-      <c r="F34" s="100"/>
+      <c r="F34" s="87"/>
       <c r="G34" s="15">
         <v>5320301</v>
       </c>
@@ -7671,7 +7668,7 @@
         <f t="shared" si="0"/>
         <v>112</v>
       </c>
-      <c r="F35" s="100"/>
+      <c r="F35" s="87"/>
       <c r="G35" s="15">
         <v>5540125</v>
       </c>
@@ -7708,7 +7705,7 @@
         <f t="shared" si="0"/>
         <v>108</v>
       </c>
-      <c r="F36" s="100"/>
+      <c r="F36" s="87"/>
       <c r="G36" s="15">
         <v>5810207</v>
       </c>
@@ -7745,7 +7742,7 @@
         <f t="shared" si="0"/>
         <v>220</v>
       </c>
-      <c r="F37" s="100"/>
+      <c r="F37" s="87"/>
       <c r="G37" s="15">
         <v>5640101</v>
       </c>
@@ -7782,7 +7779,7 @@
         <f t="shared" si="0"/>
         <v>221</v>
       </c>
-      <c r="F38" s="100"/>
+      <c r="F38" s="87"/>
       <c r="G38" s="15">
         <v>5620116</v>
       </c>
@@ -7819,7 +7816,7 @@
         <f t="shared" si="0"/>
         <v>201</v>
       </c>
-      <c r="F39" s="100"/>
+      <c r="F39" s="87"/>
       <c r="G39" s="16">
         <v>5520223</v>
       </c>
@@ -7856,7 +7853,7 @@
         <f t="shared" si="0"/>
         <v>201</v>
       </c>
-      <c r="F40" s="100"/>
+      <c r="F40" s="87"/>
       <c r="G40" s="17">
         <v>5520222</v>
       </c>
@@ -7893,7 +7890,6 @@
         <f t="shared" si="0"/>
         <v>201</v>
       </c>
-      <c r="F41" s="101"/>
       <c r="G41" s="17">
         <v>5520224</v>
       </c>
@@ -7930,7 +7926,6 @@
         <f t="shared" si="0"/>
         <v>201</v>
       </c>
-      <c r="F42" s="101"/>
     </row>
     <row r="43" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B43" s="6" t="s">
@@ -7947,7 +7942,6 @@
         <f t="shared" si="0"/>
         <v>201</v>
       </c>
-      <c r="F43" s="101"/>
     </row>
     <row r="44" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B44" s="6" t="s">
@@ -7964,7 +7958,6 @@
         <f t="shared" si="0"/>
         <v>215</v>
       </c>
-      <c r="F44" s="101"/>
     </row>
     <row r="45" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B45" s="6" t="s">
@@ -7981,7 +7974,6 @@
         <f t="shared" si="0"/>
         <v>215</v>
       </c>
-      <c r="F45" s="101"/>
     </row>
     <row r="46" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B46" s="6" t="s">
@@ -7998,7 +7990,6 @@
         <f t="shared" si="0"/>
         <v>216</v>
       </c>
-      <c r="F46" s="101"/>
     </row>
     <row r="47" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B47" s="6" t="s">
@@ -8015,7 +8006,6 @@
         <f t="shared" si="0"/>
         <v>207</v>
       </c>
-      <c r="F47" s="101"/>
     </row>
     <row r="48" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B48" s="6" t="s">
@@ -8032,9 +8022,8 @@
         <f t="shared" si="0"/>
         <v>220</v>
       </c>
-      <c r="F48" s="101"/>
-    </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B49" s="6" t="s">
         <v>116</v>
       </c>
@@ -8049,9 +8038,8 @@
         <f t="shared" si="0"/>
         <v>204</v>
       </c>
-      <c r="F49" s="101"/>
-    </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B50" s="6" t="s">
         <v>117</v>
       </c>
@@ -8066,9 +8054,8 @@
         <f t="shared" si="0"/>
         <v>204</v>
       </c>
-      <c r="F50" s="101"/>
-    </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B51" s="6" t="s">
         <v>118</v>
       </c>
@@ -8083,9 +8070,8 @@
         <f t="shared" si="0"/>
         <v>204</v>
       </c>
-      <c r="F51" s="101"/>
-    </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B52" s="6" t="s">
         <v>119</v>
       </c>
@@ -8100,9 +8086,8 @@
         <f t="shared" si="0"/>
         <v>205</v>
       </c>
-      <c r="F52" s="101"/>
-    </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B53" s="6" t="s">
         <v>120</v>
       </c>
@@ -8117,9 +8102,8 @@
         <f t="shared" si="0"/>
         <v>208</v>
       </c>
-      <c r="F53" s="101"/>
-    </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="54" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B54" s="6" t="s">
         <v>121</v>
       </c>
@@ -8134,9 +8118,8 @@
         <f t="shared" si="0"/>
         <v>209</v>
       </c>
-      <c r="F54" s="101"/>
-    </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B55" s="6" t="s">
         <v>122</v>
       </c>
@@ -8151,9 +8134,8 @@
         <f t="shared" si="0"/>
         <v>209</v>
       </c>
-      <c r="F55" s="101"/>
-    </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="56" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B56" s="6" t="s">
         <v>123</v>
       </c>
@@ -8168,9 +8150,8 @@
         <f t="shared" si="0"/>
         <v>210</v>
       </c>
-      <c r="F56" s="101"/>
-    </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="57" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B57" s="6" t="s">
         <v>124</v>
       </c>
@@ -8185,9 +8166,8 @@
         <f t="shared" si="0"/>
         <v>203</v>
       </c>
-      <c r="F57" s="101"/>
-    </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="58" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B58" s="6" t="s">
         <v>125</v>
       </c>
@@ -8202,9 +8182,8 @@
         <f t="shared" si="0"/>
         <v>217</v>
       </c>
-      <c r="F58" s="101"/>
-    </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="59" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B59" s="6" t="s">
         <v>126</v>
       </c>
@@ -8219,9 +8198,8 @@
         <f t="shared" si="0"/>
         <v>214</v>
       </c>
-      <c r="F59" s="101"/>
-    </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="60" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B60" s="6" t="s">
         <v>127</v>
       </c>
@@ -8236,9 +8214,8 @@
         <f t="shared" si="0"/>
         <v>218</v>
       </c>
-      <c r="F60" s="101"/>
-    </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="61" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B61" s="6" t="s">
         <v>128</v>
       </c>
@@ -8253,9 +8230,8 @@
         <f t="shared" si="0"/>
         <v>218</v>
       </c>
-      <c r="F61" s="101"/>
-    </row>
-    <row r="62" spans="2:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="62" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B62" s="6" t="s">
         <v>1692</v>
       </c>
@@ -8270,9 +8246,8 @@
         <f t="shared" si="0"/>
         <v>213</v>
       </c>
-      <c r="F62" s="101"/>
-    </row>
-    <row r="63" spans="2:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="63" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B63" s="6" t="s">
         <v>129</v>
       </c>
@@ -8287,9 +8262,8 @@
         <f t="shared" si="0"/>
         <v>221</v>
       </c>
-      <c r="F63" s="101"/>
-    </row>
-    <row r="64" spans="2:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="64" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B64" s="6" t="s">
         <v>130</v>
       </c>
@@ -8304,9 +8278,8 @@
         <f t="shared" ref="E64:E104" si="6">INDEX(L:L,MATCH(IF(MID(B64,3,1)="T","TC_"&amp;C64,"CĐ_"&amp;C64),J:J,0),1)</f>
         <v>221</v>
       </c>
-      <c r="F64" s="101"/>
-    </row>
-    <row r="65" spans="2:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="65" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B65" s="6" t="s">
         <v>131</v>
       </c>
@@ -8321,9 +8294,8 @@
         <f t="shared" si="6"/>
         <v>223</v>
       </c>
-      <c r="F65" s="101"/>
-    </row>
-    <row r="66" spans="2:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="66" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B66" s="6" t="s">
         <v>132</v>
       </c>
@@ -8338,9 +8310,8 @@
         <f t="shared" si="6"/>
         <v>222</v>
       </c>
-      <c r="F66" s="101"/>
-    </row>
-    <row r="67" spans="2:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="67" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B67" s="6" t="s">
         <v>133</v>
       </c>
@@ -8355,9 +8326,8 @@
         <f t="shared" si="6"/>
         <v>219</v>
       </c>
-      <c r="F67" s="101"/>
-    </row>
-    <row r="68" spans="2:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="68" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B68" s="6" t="s">
         <v>134</v>
       </c>
@@ -8372,9 +8342,8 @@
         <f t="shared" si="6"/>
         <v>101</v>
       </c>
-      <c r="F68" s="101"/>
-    </row>
-    <row r="69" spans="2:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="69" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B69" s="6" t="s">
         <v>135</v>
       </c>
@@ -8389,9 +8358,8 @@
         <f t="shared" si="6"/>
         <v>101</v>
       </c>
-      <c r="F69" s="101"/>
-    </row>
-    <row r="70" spans="2:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="70" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B70" s="6" t="s">
         <v>136</v>
       </c>
@@ -8406,9 +8374,8 @@
         <f t="shared" si="6"/>
         <v>102</v>
       </c>
-      <c r="F70" s="101"/>
-    </row>
-    <row r="71" spans="2:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="71" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B71" s="6" t="s">
         <v>137</v>
       </c>
@@ -8423,9 +8390,8 @@
         <f t="shared" si="6"/>
         <v>102</v>
       </c>
-      <c r="F71" s="101"/>
-    </row>
-    <row r="72" spans="2:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="72" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B72" s="6" t="s">
         <v>138</v>
       </c>
@@ -8440,9 +8406,8 @@
         <f t="shared" si="6"/>
         <v>106</v>
       </c>
-      <c r="F72" s="101"/>
-    </row>
-    <row r="73" spans="2:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="73" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B73" s="6" t="s">
         <v>139</v>
       </c>
@@ -8457,9 +8422,8 @@
         <f t="shared" si="6"/>
         <v>112</v>
       </c>
-      <c r="F73" s="101"/>
-    </row>
-    <row r="74" spans="2:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="74" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B74" s="6" t="s">
         <v>140</v>
       </c>
@@ -8474,9 +8438,8 @@
         <f t="shared" si="6"/>
         <v>111</v>
       </c>
-      <c r="F74" s="101"/>
-    </row>
-    <row r="75" spans="2:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="75" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B75" s="6" t="s">
         <v>141</v>
       </c>
@@ -8491,9 +8454,8 @@
         <f t="shared" si="6"/>
         <v>103</v>
       </c>
-      <c r="F75" s="101"/>
-    </row>
-    <row r="76" spans="2:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="76" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B76" s="6" t="s">
         <v>142</v>
       </c>
@@ -8508,9 +8470,8 @@
         <f t="shared" si="6"/>
         <v>104</v>
       </c>
-      <c r="F76" s="101"/>
-    </row>
-    <row r="77" spans="2:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="77" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B77" s="6" t="s">
         <v>143</v>
       </c>
@@ -8525,9 +8486,8 @@
         <f t="shared" si="6"/>
         <v>220</v>
       </c>
-      <c r="F77" s="101"/>
-    </row>
-    <row r="78" spans="2:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="78" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B78" s="6" t="s">
         <v>144</v>
       </c>
@@ -8542,9 +8502,8 @@
         <f t="shared" si="6"/>
         <v>221</v>
       </c>
-      <c r="F78" s="101"/>
-    </row>
-    <row r="79" spans="2:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="79" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B79" s="6" t="s">
         <v>1693</v>
       </c>
@@ -8559,9 +8518,8 @@
         <f t="shared" si="6"/>
         <v>201</v>
       </c>
-      <c r="F79" s="101"/>
-    </row>
-    <row r="80" spans="2:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="80" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B80" s="6" t="s">
         <v>1694</v>
       </c>
@@ -8576,9 +8534,8 @@
         <f t="shared" si="6"/>
         <v>201</v>
       </c>
-      <c r="F80" s="101"/>
-    </row>
-    <row r="81" spans="2:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="81" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B81" s="6" t="s">
         <v>1695</v>
       </c>
@@ -8593,9 +8550,8 @@
         <f t="shared" si="6"/>
         <v>201</v>
       </c>
-      <c r="F81" s="101"/>
-    </row>
-    <row r="82" spans="2:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="82" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B82" s="6" t="s">
         <v>1696</v>
       </c>
@@ -8610,9 +8566,8 @@
         <f t="shared" si="6"/>
         <v>201</v>
       </c>
-      <c r="F82" s="101"/>
-    </row>
-    <row r="83" spans="2:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="83" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B83" s="6" t="s">
         <v>1697</v>
       </c>
@@ -8627,9 +8582,8 @@
         <f t="shared" si="6"/>
         <v>204</v>
       </c>
-      <c r="F83" s="101"/>
-    </row>
-    <row r="84" spans="2:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="84" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B84" s="6" t="s">
         <v>1698</v>
       </c>
@@ -8644,9 +8598,8 @@
         <f t="shared" si="6"/>
         <v>205</v>
       </c>
-      <c r="F84" s="101"/>
-    </row>
-    <row r="85" spans="2:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="85" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B85" s="6" t="s">
         <v>1699</v>
       </c>
@@ -8661,9 +8614,8 @@
         <f t="shared" si="6"/>
         <v>219</v>
       </c>
-      <c r="F85" s="101"/>
-    </row>
-    <row r="86" spans="2:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="86" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B86" s="6" t="s">
         <v>1700</v>
       </c>
@@ -8678,9 +8630,8 @@
         <f t="shared" si="6"/>
         <v>222</v>
       </c>
-      <c r="F86" s="101"/>
-    </row>
-    <row r="87" spans="2:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="87" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B87" s="6" t="s">
         <v>1701</v>
       </c>
@@ -8695,9 +8646,8 @@
         <f t="shared" si="6"/>
         <v>224</v>
       </c>
-      <c r="F87" s="101"/>
-    </row>
-    <row r="88" spans="2:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="88" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B88" s="6" t="s">
         <v>1702</v>
       </c>
@@ -8712,9 +8662,8 @@
         <f t="shared" si="6"/>
         <v>217</v>
       </c>
-      <c r="F88" s="101"/>
-    </row>
-    <row r="89" spans="2:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="89" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B89" s="6" t="s">
         <v>1703</v>
       </c>
@@ -8729,9 +8678,8 @@
         <f t="shared" si="6"/>
         <v>209</v>
       </c>
-      <c r="F89" s="101"/>
-    </row>
-    <row r="90" spans="2:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="90" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B90" s="6" t="s">
         <v>1704</v>
       </c>
@@ -8746,9 +8694,8 @@
         <f t="shared" si="6"/>
         <v>209</v>
       </c>
-      <c r="F90" s="101"/>
-    </row>
-    <row r="91" spans="2:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="91" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B91" s="6" t="s">
         <v>1705</v>
       </c>
@@ -8763,9 +8710,8 @@
         <f t="shared" si="6"/>
         <v>210</v>
       </c>
-      <c r="F91" s="101"/>
-    </row>
-    <row r="92" spans="2:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="92" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B92" s="6" t="s">
         <v>1706</v>
       </c>
@@ -8780,9 +8726,8 @@
         <f t="shared" si="6"/>
         <v>213</v>
       </c>
-      <c r="F92" s="101"/>
-    </row>
-    <row r="93" spans="2:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="93" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B93" s="6" t="s">
         <v>1707</v>
       </c>
@@ -8797,9 +8742,8 @@
         <f t="shared" si="6"/>
         <v>213</v>
       </c>
-      <c r="F93" s="101"/>
-    </row>
-    <row r="94" spans="2:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="94" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B94" s="6" t="s">
         <v>1708</v>
       </c>
@@ -8814,9 +8758,8 @@
         <f t="shared" si="6"/>
         <v>218</v>
       </c>
-      <c r="F94" s="101"/>
-    </row>
-    <row r="95" spans="2:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="95" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B95" s="6" t="s">
         <v>1709</v>
       </c>
@@ -8831,9 +8774,8 @@
         <f t="shared" si="6"/>
         <v>214</v>
       </c>
-      <c r="F95" s="101"/>
-    </row>
-    <row r="96" spans="2:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="96" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B96" s="6" t="s">
         <v>1710</v>
       </c>
@@ -8848,9 +8790,8 @@
         <f t="shared" si="6"/>
         <v>221</v>
       </c>
-      <c r="F96" s="101"/>
-    </row>
-    <row r="97" spans="2:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="97" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B97" s="6" t="s">
         <v>1711</v>
       </c>
@@ -8865,9 +8806,8 @@
         <f t="shared" si="6"/>
         <v>221</v>
       </c>
-      <c r="F97" s="101"/>
-    </row>
-    <row r="98" spans="2:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="98" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B98" s="6" t="s">
         <v>1712</v>
       </c>
@@ -8882,9 +8822,8 @@
         <f t="shared" si="6"/>
         <v>215</v>
       </c>
-      <c r="F98" s="101"/>
-    </row>
-    <row r="99" spans="2:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="99" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B99" s="6" t="s">
         <v>1713</v>
       </c>
@@ -8899,9 +8838,8 @@
         <f t="shared" si="6"/>
         <v>201</v>
       </c>
-      <c r="F99" s="101"/>
-    </row>
-    <row r="100" spans="2:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="100" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B100" s="80" t="s">
         <v>1714</v>
       </c>
@@ -8916,9 +8854,8 @@
         <f t="shared" si="6"/>
         <v>207</v>
       </c>
-      <c r="F100" s="101"/>
-    </row>
-    <row r="101" spans="2:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="101" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B101" s="6" t="s">
         <v>1715</v>
       </c>
@@ -8933,9 +8870,8 @@
         <f t="shared" si="6"/>
         <v>204</v>
       </c>
-      <c r="F101" s="101"/>
-    </row>
-    <row r="102" spans="2:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="102" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B102" s="6" t="s">
         <v>1719</v>
       </c>
@@ -8950,9 +8886,8 @@
         <f t="shared" si="6"/>
         <v>101</v>
       </c>
-      <c r="F102" s="101"/>
-    </row>
-    <row r="103" spans="2:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="103" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B103" s="6" t="s">
         <v>1720</v>
       </c>
@@ -8960,16 +8895,15 @@
         <v>15</v>
       </c>
       <c r="D103" s="7" t="str">
-        <f t="shared" ref="D79:D103" si="8">UPPER(INDEX(I:I,MATCH(C103,H:H,0),1))</f>
+        <f t="shared" ref="D103" si="8">UPPER(INDEX(I:I,MATCH(C103,H:H,0),1))</f>
         <v>CÔNG NGHỆ KỸ THUẬT Ô TÔ</v>
       </c>
       <c r="E103" s="8" t="str">
         <f t="shared" si="6"/>
         <v>102</v>
       </c>
-      <c r="F103" s="101"/>
-    </row>
-    <row r="104" spans="2:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="104" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B104" s="6" t="s">
         <v>1721</v>
       </c>
@@ -8984,9 +8918,8 @@
         <f t="shared" si="6"/>
         <v>101</v>
       </c>
-      <c r="F104" s="101"/>
-    </row>
-    <row r="105" spans="2:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="105" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B105" s="6" t="s">
         <v>1718</v>
       </c>
@@ -8998,12 +8931,11 @@
         <v>CÔNG NGHỆ KỸ THUẬT Ô TÔ</v>
       </c>
       <c r="E105" s="8" t="str">
-        <f t="shared" ref="E98:E114" si="10">INDEX(L:L,MATCH(IF(MID(B105,3,1)="T","TC_"&amp;C105,"CĐ_"&amp;C105),J:J,0),1)</f>
+        <f t="shared" ref="E105:E114" si="10">INDEX(L:L,MATCH(IF(MID(B105,3,1)="T","TC_"&amp;C105,"CĐ_"&amp;C105),J:J,0),1)</f>
         <v>102</v>
       </c>
-      <c r="F105" s="101"/>
-    </row>
-    <row r="106" spans="2:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="106" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B106" s="6" t="s">
         <v>1722</v>
       </c>
@@ -9018,9 +8950,8 @@
         <f t="shared" si="10"/>
         <v>111</v>
       </c>
-      <c r="F106" s="101"/>
-    </row>
-    <row r="107" spans="2:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="107" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B107" s="6" t="s">
         <v>1723</v>
       </c>
@@ -9035,9 +8966,8 @@
         <f t="shared" si="10"/>
         <v>111</v>
       </c>
-      <c r="F107" s="101"/>
-    </row>
-    <row r="108" spans="2:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="108" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B108" s="6" t="s">
         <v>1724</v>
       </c>
@@ -9052,9 +8982,8 @@
         <f t="shared" si="10"/>
         <v>112</v>
       </c>
-      <c r="F108" s="101"/>
-    </row>
-    <row r="109" spans="2:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="109" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B109" s="6" t="s">
         <v>1725</v>
       </c>
@@ -9069,9 +8998,8 @@
         <f t="shared" si="10"/>
         <v>103</v>
       </c>
-      <c r="F109" s="101"/>
-    </row>
-    <row r="110" spans="2:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="110" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B110" s="6" t="s">
         <v>1726</v>
       </c>
@@ -9086,9 +9014,8 @@
         <f t="shared" si="10"/>
         <v>108</v>
       </c>
-      <c r="F110" s="101"/>
-    </row>
-    <row r="111" spans="2:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="111" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B111" s="6" t="s">
         <v>1727</v>
       </c>
@@ -9103,9 +9030,8 @@
         <f t="shared" si="10"/>
         <v>104</v>
       </c>
-      <c r="F111" s="101"/>
-    </row>
-    <row r="112" spans="2:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="112" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B112" s="6" t="s">
         <v>1728</v>
       </c>
@@ -9120,7 +9046,6 @@
         <f t="shared" si="10"/>
         <v>106</v>
       </c>
-      <c r="F112" s="101"/>
     </row>
     <row r="113" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B113" s="83" t="s">
@@ -9137,7 +9062,7 @@
         <f t="shared" si="10"/>
         <v>110</v>
       </c>
-      <c r="F113" s="102"/>
+      <c r="F113" s="88"/>
     </row>
     <row r="114" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B114" s="6" t="s">
@@ -9154,7 +9079,6 @@
         <f t="shared" si="10"/>
         <v>109</v>
       </c>
-      <c r="F114" s="101"/>
     </row>
     <row r="122" spans="2:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
@@ -17321,25 +17245,25 @@
       <c r="E67" s="49"/>
     </row>
     <row r="68" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="89">
+      <c r="A68" s="90">
         <v>5210305</v>
       </c>
-      <c r="B68" s="89" t="s">
+      <c r="B68" s="90" t="s">
         <v>689</v>
       </c>
-      <c r="C68" s="89">
+      <c r="C68" s="90">
         <v>6210305</v>
       </c>
-      <c r="D68" s="89" t="s">
+      <c r="D68" s="90" t="s">
         <v>689</v>
       </c>
       <c r="E68" s="66"/>
     </row>
     <row r="69" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="90"/>
-      <c r="B69" s="90"/>
-      <c r="C69" s="90"/>
-      <c r="D69" s="90"/>
+      <c r="A69" s="91"/>
+      <c r="B69" s="91"/>
+      <c r="C69" s="91"/>
+      <c r="D69" s="91"/>
       <c r="E69" s="49"/>
     </row>
     <row r="70" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -20335,30 +20259,30 @@
       <c r="E229" s="49"/>
     </row>
     <row r="230" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A230" s="89">
+      <c r="A230" s="90">
         <v>5340410</v>
       </c>
       <c r="B230" s="69" t="s">
         <v>849</v>
       </c>
-      <c r="C230" s="89">
+      <c r="C230" s="90">
         <v>6340410</v>
       </c>
       <c r="D230" s="70" t="s">
         <v>849</v>
       </c>
-      <c r="E230" s="96"/>
+      <c r="E230" s="92"/>
     </row>
     <row r="231" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A231" s="90"/>
+      <c r="A231" s="91"/>
       <c r="B231" s="48" t="s">
         <v>850</v>
       </c>
-      <c r="C231" s="90"/>
+      <c r="C231" s="91"/>
       <c r="D231" s="48" t="s">
         <v>850</v>
       </c>
-      <c r="E231" s="97"/>
+      <c r="E231" s="93"/>
     </row>
     <row r="232" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A232" s="47">
@@ -20406,30 +20330,30 @@
       <c r="E234" s="49"/>
     </row>
     <row r="235" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A235" s="89">
+      <c r="A235" s="90">
         <v>5340414</v>
       </c>
       <c r="B235" s="69" t="s">
         <v>856</v>
       </c>
-      <c r="C235" s="89">
+      <c r="C235" s="90">
         <v>6340414</v>
       </c>
       <c r="D235" s="70" t="s">
         <v>856</v>
       </c>
-      <c r="E235" s="96"/>
+      <c r="E235" s="92"/>
     </row>
     <row r="236" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A236" s="90"/>
+      <c r="A236" s="91"/>
       <c r="B236" s="48" t="s">
         <v>857</v>
       </c>
-      <c r="C236" s="90"/>
+      <c r="C236" s="91"/>
       <c r="D236" s="48" t="s">
         <v>857</v>
       </c>
-      <c r="E236" s="97"/>
+      <c r="E236" s="93"/>
     </row>
     <row r="237" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A237" s="47">
@@ -21906,28 +21830,28 @@
       <c r="E342" s="49"/>
     </row>
     <row r="343" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A343" s="89">
+      <c r="A343" s="90">
         <v>5510105</v>
       </c>
-      <c r="B343" s="89" t="s">
+      <c r="B343" s="90" t="s">
         <v>954</v>
       </c>
-      <c r="C343" s="89">
+      <c r="C343" s="90">
         <v>6510105</v>
       </c>
       <c r="D343" s="69" t="s">
         <v>955</v>
       </c>
-      <c r="E343" s="96"/>
+      <c r="E343" s="92"/>
     </row>
     <row r="344" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A344" s="90"/>
-      <c r="B344" s="90"/>
-      <c r="C344" s="90"/>
+      <c r="A344" s="91"/>
+      <c r="B344" s="91"/>
+      <c r="C344" s="91"/>
       <c r="D344" s="48" t="s">
         <v>954</v>
       </c>
-      <c r="E344" s="97"/>
+      <c r="E344" s="93"/>
     </row>
     <row r="345" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A345" s="47">
@@ -22369,28 +22293,28 @@
       <c r="E377" s="49"/>
     </row>
     <row r="378" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A378" s="89">
+      <c r="A378" s="90">
         <v>5510215</v>
       </c>
-      <c r="B378" s="89" t="s">
+      <c r="B378" s="90" t="s">
         <v>986</v>
       </c>
-      <c r="C378" s="89">
+      <c r="C378" s="90">
         <v>6510215</v>
       </c>
       <c r="D378" s="69" t="s">
         <v>987</v>
       </c>
-      <c r="E378" s="96"/>
+      <c r="E378" s="92"/>
     </row>
     <row r="379" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A379" s="90"/>
-      <c r="B379" s="90"/>
-      <c r="C379" s="90"/>
+      <c r="A379" s="91"/>
+      <c r="B379" s="91"/>
+      <c r="C379" s="91"/>
       <c r="D379" s="48" t="s">
         <v>988</v>
       </c>
-      <c r="E379" s="97"/>
+      <c r="E379" s="93"/>
     </row>
     <row r="380" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A380" s="47">
@@ -22585,52 +22509,52 @@
       <c r="E395" s="49"/>
     </row>
     <row r="396" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A396" s="89">
+      <c r="A396" s="90">
         <v>5510312</v>
       </c>
-      <c r="B396" s="89" t="s">
+      <c r="B396" s="90" t="s">
         <v>1004</v>
       </c>
-      <c r="C396" s="89">
+      <c r="C396" s="90">
         <v>6510312</v>
       </c>
       <c r="D396" s="70" t="s">
         <v>1005</v>
       </c>
-      <c r="E396" s="96"/>
+      <c r="E396" s="92"/>
     </row>
     <row r="397" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A397" s="90"/>
-      <c r="B397" s="90"/>
-      <c r="C397" s="90"/>
+      <c r="A397" s="91"/>
+      <c r="B397" s="91"/>
+      <c r="C397" s="91"/>
       <c r="D397" s="48" t="s">
         <v>1006</v>
       </c>
-      <c r="E397" s="97"/>
+      <c r="E397" s="93"/>
     </row>
     <row r="398" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A398" s="89">
+      <c r="A398" s="90">
         <v>5510313</v>
       </c>
-      <c r="B398" s="98" t="s">
+      <c r="B398" s="94" t="s">
         <v>1007</v>
       </c>
-      <c r="C398" s="89">
+      <c r="C398" s="90">
         <v>6510313</v>
       </c>
       <c r="D398" s="70" t="s">
         <v>1008</v>
       </c>
-      <c r="E398" s="96"/>
+      <c r="E398" s="92"/>
     </row>
     <row r="399" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A399" s="90"/>
-      <c r="B399" s="99"/>
-      <c r="C399" s="90"/>
+      <c r="A399" s="91"/>
+      <c r="B399" s="95"/>
+      <c r="C399" s="91"/>
       <c r="D399" s="48" t="s">
         <v>1009</v>
       </c>
-      <c r="E399" s="97"/>
+      <c r="E399" s="93"/>
     </row>
     <row r="400" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A400" s="47">
@@ -22648,28 +22572,28 @@
       <c r="E400" s="49"/>
     </row>
     <row r="401" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A401" s="89">
+      <c r="A401" s="90">
         <v>5510315</v>
       </c>
-      <c r="B401" s="98" t="s">
+      <c r="B401" s="94" t="s">
         <v>1011</v>
       </c>
-      <c r="C401" s="89">
+      <c r="C401" s="90">
         <v>6510315</v>
       </c>
       <c r="D401" s="70" t="s">
         <v>1012</v>
       </c>
-      <c r="E401" s="96"/>
+      <c r="E401" s="92"/>
     </row>
     <row r="402" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A402" s="90"/>
-      <c r="B402" s="99"/>
-      <c r="C402" s="90"/>
+      <c r="A402" s="91"/>
+      <c r="B402" s="95"/>
+      <c r="C402" s="91"/>
       <c r="D402" s="48" t="s">
         <v>1013</v>
       </c>
-      <c r="E402" s="97"/>
+      <c r="E402" s="93"/>
     </row>
     <row r="403" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A403" s="40">
@@ -25432,28 +25356,28 @@
       <c r="E602" s="49"/>
     </row>
     <row r="603" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A603" s="89">
+      <c r="A603" s="90">
         <v>5520147</v>
       </c>
-      <c r="B603" s="89" t="s">
+      <c r="B603" s="90" t="s">
         <v>1205</v>
       </c>
-      <c r="C603" s="89">
+      <c r="C603" s="90">
         <v>6520147</v>
       </c>
       <c r="D603" s="69" t="s">
         <v>1206</v>
       </c>
-      <c r="E603" s="96"/>
+      <c r="E603" s="92"/>
     </row>
     <row r="604" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A604" s="90"/>
-      <c r="B604" s="90"/>
-      <c r="C604" s="90"/>
+      <c r="A604" s="91"/>
+      <c r="B604" s="91"/>
+      <c r="C604" s="91"/>
       <c r="D604" s="48" t="s">
         <v>1207</v>
       </c>
-      <c r="E604" s="97"/>
+      <c r="E604" s="93"/>
     </row>
     <row r="605" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A605" s="47">
@@ -25530,28 +25454,28 @@
       <c r="E610" s="49"/>
     </row>
     <row r="611" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A611" s="89">
+      <c r="A611" s="90">
         <v>5520154</v>
       </c>
-      <c r="B611" s="98" t="s">
+      <c r="B611" s="94" t="s">
         <v>1214</v>
       </c>
-      <c r="C611" s="89">
+      <c r="C611" s="90">
         <v>6520154</v>
       </c>
       <c r="D611" s="69" t="s">
         <v>1215</v>
       </c>
-      <c r="E611" s="96"/>
+      <c r="E611" s="92"/>
     </row>
     <row r="612" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A612" s="90"/>
-      <c r="B612" s="99"/>
-      <c r="C612" s="90"/>
+      <c r="A612" s="91"/>
+      <c r="B612" s="95"/>
+      <c r="C612" s="91"/>
       <c r="D612" s="48" t="s">
         <v>1216</v>
       </c>
-      <c r="E612" s="97"/>
+      <c r="E612" s="93"/>
     </row>
     <row r="613" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A613" s="47">
@@ -25933,25 +25857,25 @@
       <c r="E645" s="49"/>
     </row>
     <row r="646" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A646" s="89">
+      <c r="A646" s="90">
         <v>5520184</v>
       </c>
-      <c r="B646" s="89" t="s">
+      <c r="B646" s="90" t="s">
         <v>1246</v>
       </c>
-      <c r="C646" s="89">
+      <c r="C646" s="90">
         <v>6520184</v>
       </c>
-      <c r="D646" s="89" t="s">
+      <c r="D646" s="90" t="s">
         <v>1246</v>
       </c>
       <c r="E646" s="66"/>
     </row>
     <row r="647" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A647" s="90"/>
-      <c r="B647" s="90"/>
-      <c r="C647" s="90"/>
-      <c r="D647" s="90"/>
+      <c r="A647" s="91"/>
+      <c r="B647" s="91"/>
+      <c r="C647" s="91"/>
+      <c r="D647" s="91"/>
       <c r="E647" s="49"/>
     </row>
     <row r="648" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -26803,35 +26727,35 @@
       <c r="E709" s="49"/>
     </row>
     <row r="710" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A710" s="89">
+      <c r="A710" s="90">
         <v>5520243</v>
       </c>
-      <c r="B710" s="89" t="s">
+      <c r="B710" s="90" t="s">
         <v>1307</v>
       </c>
-      <c r="C710" s="89">
+      <c r="C710" s="90">
         <v>6520243</v>
       </c>
-      <c r="D710" s="89" t="s">
+      <c r="D710" s="90" t="s">
         <v>1307</v>
       </c>
       <c r="E710" s="66"/>
     </row>
     <row r="711" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A711" s="90"/>
-      <c r="B711" s="90"/>
-      <c r="C711" s="90"/>
-      <c r="D711" s="90"/>
+      <c r="A711" s="91"/>
+      <c r="B711" s="91"/>
+      <c r="C711" s="91"/>
+      <c r="D711" s="91"/>
       <c r="E711" s="49"/>
     </row>
     <row r="712" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A712" s="89">
+      <c r="A712" s="90">
         <v>5520244</v>
       </c>
-      <c r="B712" s="89" t="s">
+      <c r="B712" s="90" t="s">
         <v>1308</v>
       </c>
-      <c r="C712" s="89">
+      <c r="C712" s="90">
         <v>6520244</v>
       </c>
       <c r="D712" s="69" t="s">
@@ -26840,18 +26764,18 @@
       <c r="E712" s="66"/>
     </row>
     <row r="713" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A713" s="95"/>
-      <c r="B713" s="95"/>
-      <c r="C713" s="95"/>
+      <c r="A713" s="98"/>
+      <c r="B713" s="98"/>
+      <c r="C713" s="98"/>
       <c r="D713" s="69" t="s">
         <v>1310</v>
       </c>
       <c r="E713" s="66"/>
     </row>
     <row r="714" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A714" s="90"/>
-      <c r="B714" s="90"/>
-      <c r="C714" s="90"/>
+      <c r="A714" s="91"/>
+      <c r="B714" s="91"/>
+      <c r="C714" s="91"/>
       <c r="D714" s="74"/>
       <c r="E714" s="49"/>
     </row>
@@ -26964,25 +26888,25 @@
       <c r="E722" s="49"/>
     </row>
     <row r="723" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A723" s="89">
+      <c r="A723" s="90">
         <v>5520251</v>
       </c>
-      <c r="B723" s="89" t="s">
+      <c r="B723" s="90" t="s">
         <v>1317</v>
       </c>
-      <c r="C723" s="89">
+      <c r="C723" s="90">
         <v>6520251</v>
       </c>
-      <c r="D723" s="89" t="s">
+      <c r="D723" s="90" t="s">
         <v>1317</v>
       </c>
       <c r="E723" s="66"/>
     </row>
     <row r="724" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A724" s="90"/>
-      <c r="B724" s="90"/>
-      <c r="C724" s="90"/>
-      <c r="D724" s="90"/>
+      <c r="A724" s="91"/>
+      <c r="B724" s="91"/>
+      <c r="C724" s="91"/>
+      <c r="D724" s="91"/>
       <c r="E724" s="49"/>
     </row>
     <row r="725" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -28159,25 +28083,25 @@
       <c r="E811" s="49"/>
     </row>
     <row r="812" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A812" s="91">
+      <c r="A812" s="99">
         <v>55402</v>
       </c>
-      <c r="B812" s="91" t="s">
+      <c r="B812" s="99" t="s">
         <v>1399</v>
       </c>
-      <c r="C812" s="91">
+      <c r="C812" s="99">
         <v>65402</v>
       </c>
-      <c r="D812" s="91" t="s">
+      <c r="D812" s="99" t="s">
         <v>1399</v>
       </c>
       <c r="E812" s="75"/>
     </row>
     <row r="813" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A813" s="92"/>
-      <c r="B813" s="92"/>
-      <c r="C813" s="92"/>
-      <c r="D813" s="92"/>
+      <c r="A813" s="100"/>
+      <c r="B813" s="100"/>
+      <c r="C813" s="100"/>
+      <c r="D813" s="100"/>
       <c r="E813" s="42"/>
     </row>
     <row r="814" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -28660,21 +28584,21 @@
       <c r="E850" s="49"/>
     </row>
     <row r="851" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A851" s="89">
+      <c r="A851" s="90">
         <v>5580209</v>
       </c>
-      <c r="B851" s="89" t="s">
+      <c r="B851" s="90" t="s">
         <v>1433</v>
       </c>
-      <c r="C851" s="93"/>
-      <c r="D851" s="93"/>
+      <c r="C851" s="96"/>
+      <c r="D851" s="96"/>
       <c r="E851" s="66"/>
     </row>
     <row r="852" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A852" s="90"/>
-      <c r="B852" s="90"/>
-      <c r="C852" s="94"/>
-      <c r="D852" s="94"/>
+      <c r="A852" s="91"/>
+      <c r="B852" s="91"/>
+      <c r="C852" s="97"/>
+      <c r="D852" s="97"/>
       <c r="E852" s="49"/>
     </row>
     <row r="853" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -29075,25 +28999,25 @@
       <c r="E883" s="49"/>
     </row>
     <row r="884" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A884" s="89">
+      <c r="A884" s="90">
         <v>5620123</v>
       </c>
-      <c r="B884" s="89" t="s">
+      <c r="B884" s="90" t="s">
         <v>1462</v>
       </c>
-      <c r="C884" s="89">
+      <c r="C884" s="90">
         <v>6620123</v>
       </c>
-      <c r="D884" s="89" t="s">
+      <c r="D884" s="90" t="s">
         <v>1462</v>
       </c>
       <c r="E884" s="66"/>
     </row>
     <row r="885" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A885" s="90"/>
-      <c r="B885" s="90"/>
-      <c r="C885" s="90"/>
-      <c r="D885" s="90"/>
+      <c r="A885" s="91"/>
+      <c r="B885" s="91"/>
+      <c r="C885" s="91"/>
+      <c r="D885" s="91"/>
       <c r="E885" s="49"/>
     </row>
     <row r="886" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -31273,28 +31197,28 @@
       <c r="E1045" s="49"/>
     </row>
     <row r="1046" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1046" s="91">
+      <c r="A1046" s="99">
         <v>58402</v>
       </c>
-      <c r="B1046" s="91" t="s">
+      <c r="B1046" s="99" t="s">
         <v>1611</v>
       </c>
-      <c r="C1046" s="91">
+      <c r="C1046" s="99">
         <v>68402</v>
       </c>
       <c r="D1046" s="69" t="s">
         <v>1612</v>
       </c>
-      <c r="E1046" s="87"/>
+      <c r="E1046" s="101"/>
     </row>
     <row r="1047" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1047" s="92"/>
-      <c r="B1047" s="92"/>
-      <c r="C1047" s="92"/>
+      <c r="A1047" s="100"/>
+      <c r="B1047" s="100"/>
+      <c r="C1047" s="100"/>
       <c r="D1047" s="41" t="s">
         <v>1611</v>
       </c>
-      <c r="E1047" s="88"/>
+      <c r="E1047" s="102"/>
     </row>
     <row r="1048" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1048" s="47">
@@ -32380,52 +32304,14 @@
     </row>
   </sheetData>
   <mergeCells count="69">
-    <mergeCell ref="A68:A69"/>
-    <mergeCell ref="B68:B69"/>
-    <mergeCell ref="C68:C69"/>
-    <mergeCell ref="D68:D69"/>
-    <mergeCell ref="A230:A231"/>
-    <mergeCell ref="C230:C231"/>
-    <mergeCell ref="E230:E231"/>
-    <mergeCell ref="A235:A236"/>
-    <mergeCell ref="C235:C236"/>
-    <mergeCell ref="E235:E236"/>
-    <mergeCell ref="A343:A344"/>
-    <mergeCell ref="B343:B344"/>
-    <mergeCell ref="C343:C344"/>
-    <mergeCell ref="E343:E344"/>
-    <mergeCell ref="A378:A379"/>
-    <mergeCell ref="B378:B379"/>
-    <mergeCell ref="C378:C379"/>
-    <mergeCell ref="E378:E379"/>
-    <mergeCell ref="A396:A397"/>
-    <mergeCell ref="B396:B397"/>
-    <mergeCell ref="C396:C397"/>
-    <mergeCell ref="E396:E397"/>
-    <mergeCell ref="A398:A399"/>
-    <mergeCell ref="B398:B399"/>
-    <mergeCell ref="C398:C399"/>
-    <mergeCell ref="E398:E399"/>
-    <mergeCell ref="A401:A402"/>
-    <mergeCell ref="B401:B402"/>
-    <mergeCell ref="C401:C402"/>
-    <mergeCell ref="E401:E402"/>
-    <mergeCell ref="A603:A604"/>
-    <mergeCell ref="B603:B604"/>
-    <mergeCell ref="C603:C604"/>
-    <mergeCell ref="E603:E604"/>
-    <mergeCell ref="A611:A612"/>
-    <mergeCell ref="B611:B612"/>
-    <mergeCell ref="C611:C612"/>
-    <mergeCell ref="E611:E612"/>
-    <mergeCell ref="A646:A647"/>
-    <mergeCell ref="B646:B647"/>
-    <mergeCell ref="C646:C647"/>
-    <mergeCell ref="D646:D647"/>
-    <mergeCell ref="A710:A711"/>
-    <mergeCell ref="B710:B711"/>
-    <mergeCell ref="C710:C711"/>
-    <mergeCell ref="D710:D711"/>
+    <mergeCell ref="E1046:E1047"/>
+    <mergeCell ref="A884:A885"/>
+    <mergeCell ref="B884:B885"/>
+    <mergeCell ref="C884:C885"/>
+    <mergeCell ref="D884:D885"/>
+    <mergeCell ref="A1046:A1047"/>
+    <mergeCell ref="B1046:B1047"/>
+    <mergeCell ref="C1046:C1047"/>
     <mergeCell ref="A851:A852"/>
     <mergeCell ref="B851:B852"/>
     <mergeCell ref="C851:C852"/>
@@ -32441,14 +32327,52 @@
     <mergeCell ref="B812:B813"/>
     <mergeCell ref="C812:C813"/>
     <mergeCell ref="D812:D813"/>
-    <mergeCell ref="E1046:E1047"/>
-    <mergeCell ref="A884:A885"/>
-    <mergeCell ref="B884:B885"/>
-    <mergeCell ref="C884:C885"/>
-    <mergeCell ref="D884:D885"/>
-    <mergeCell ref="A1046:A1047"/>
-    <mergeCell ref="B1046:B1047"/>
-    <mergeCell ref="C1046:C1047"/>
+    <mergeCell ref="A646:A647"/>
+    <mergeCell ref="B646:B647"/>
+    <mergeCell ref="C646:C647"/>
+    <mergeCell ref="D646:D647"/>
+    <mergeCell ref="A710:A711"/>
+    <mergeCell ref="B710:B711"/>
+    <mergeCell ref="C710:C711"/>
+    <mergeCell ref="D710:D711"/>
+    <mergeCell ref="A603:A604"/>
+    <mergeCell ref="B603:B604"/>
+    <mergeCell ref="C603:C604"/>
+    <mergeCell ref="E603:E604"/>
+    <mergeCell ref="A611:A612"/>
+    <mergeCell ref="B611:B612"/>
+    <mergeCell ref="C611:C612"/>
+    <mergeCell ref="E611:E612"/>
+    <mergeCell ref="A398:A399"/>
+    <mergeCell ref="B398:B399"/>
+    <mergeCell ref="C398:C399"/>
+    <mergeCell ref="E398:E399"/>
+    <mergeCell ref="A401:A402"/>
+    <mergeCell ref="B401:B402"/>
+    <mergeCell ref="C401:C402"/>
+    <mergeCell ref="E401:E402"/>
+    <mergeCell ref="A378:A379"/>
+    <mergeCell ref="B378:B379"/>
+    <mergeCell ref="C378:C379"/>
+    <mergeCell ref="E378:E379"/>
+    <mergeCell ref="A396:A397"/>
+    <mergeCell ref="B396:B397"/>
+    <mergeCell ref="C396:C397"/>
+    <mergeCell ref="E396:E397"/>
+    <mergeCell ref="E230:E231"/>
+    <mergeCell ref="A235:A236"/>
+    <mergeCell ref="C235:C236"/>
+    <mergeCell ref="E235:E236"/>
+    <mergeCell ref="A343:A344"/>
+    <mergeCell ref="B343:B344"/>
+    <mergeCell ref="C343:C344"/>
+    <mergeCell ref="E343:E344"/>
+    <mergeCell ref="A68:A69"/>
+    <mergeCell ref="B68:B69"/>
+    <mergeCell ref="C68:C69"/>
+    <mergeCell ref="D68:D69"/>
+    <mergeCell ref="A230:A231"/>
+    <mergeCell ref="C230:C231"/>
   </mergeCells>
   <conditionalFormatting sqref="G4:H9">
     <cfRule type="duplicateValues" dxfId="7" priority="8"/>

</xml_diff>

<commit_message>
Refactor database files by updating DS_LOP_(Mau).xlsx and removing unused Danh_muc.xlsx
</commit_message>
<xml_diff>
--- a/data_base/DS_LOP_(Mau).xlsx
+++ b/data_base/DS_LOP_(Mau).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sumik\Downloads\ke-khai-gio-day-app-master\data_base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EFC94E4-D914-4F07-B8E8-AA3304244327}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69511399-58BC-4D8D-ACE0-4F3EAB9ED70F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9BE4D872-0846-4818-A986-007578B8C884}"/>
   </bookViews>
@@ -5967,10 +5967,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -5984,27 +6005,6 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -6381,8 +6381,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:L122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I110" sqref="I110"/>
+    <sheetView tabSelected="1" topLeftCell="C4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -17245,25 +17245,25 @@
       <c r="E67" s="49"/>
     </row>
     <row r="68" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="90">
+      <c r="A68" s="92">
         <v>5210305</v>
       </c>
-      <c r="B68" s="90" t="s">
+      <c r="B68" s="92" t="s">
         <v>689</v>
       </c>
-      <c r="C68" s="90">
+      <c r="C68" s="92">
         <v>6210305</v>
       </c>
-      <c r="D68" s="90" t="s">
+      <c r="D68" s="92" t="s">
         <v>689</v>
       </c>
       <c r="E68" s="66"/>
     </row>
     <row r="69" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="91"/>
-      <c r="B69" s="91"/>
-      <c r="C69" s="91"/>
-      <c r="D69" s="91"/>
+      <c r="A69" s="93"/>
+      <c r="B69" s="93"/>
+      <c r="C69" s="93"/>
+      <c r="D69" s="93"/>
       <c r="E69" s="49"/>
     </row>
     <row r="70" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -20259,30 +20259,30 @@
       <c r="E229" s="49"/>
     </row>
     <row r="230" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A230" s="90">
+      <c r="A230" s="92">
         <v>5340410</v>
       </c>
       <c r="B230" s="69" t="s">
         <v>849</v>
       </c>
-      <c r="C230" s="90">
+      <c r="C230" s="92">
         <v>6340410</v>
       </c>
       <c r="D230" s="70" t="s">
         <v>849</v>
       </c>
-      <c r="E230" s="92"/>
+      <c r="E230" s="99"/>
     </row>
     <row r="231" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A231" s="91"/>
+      <c r="A231" s="93"/>
       <c r="B231" s="48" t="s">
         <v>850</v>
       </c>
-      <c r="C231" s="91"/>
+      <c r="C231" s="93"/>
       <c r="D231" s="48" t="s">
         <v>850</v>
       </c>
-      <c r="E231" s="93"/>
+      <c r="E231" s="100"/>
     </row>
     <row r="232" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A232" s="47">
@@ -20330,30 +20330,30 @@
       <c r="E234" s="49"/>
     </row>
     <row r="235" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A235" s="90">
+      <c r="A235" s="92">
         <v>5340414</v>
       </c>
       <c r="B235" s="69" t="s">
         <v>856</v>
       </c>
-      <c r="C235" s="90">
+      <c r="C235" s="92">
         <v>6340414</v>
       </c>
       <c r="D235" s="70" t="s">
         <v>856</v>
       </c>
-      <c r="E235" s="92"/>
+      <c r="E235" s="99"/>
     </row>
     <row r="236" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A236" s="91"/>
+      <c r="A236" s="93"/>
       <c r="B236" s="48" t="s">
         <v>857</v>
       </c>
-      <c r="C236" s="91"/>
+      <c r="C236" s="93"/>
       <c r="D236" s="48" t="s">
         <v>857</v>
       </c>
-      <c r="E236" s="93"/>
+      <c r="E236" s="100"/>
     </row>
     <row r="237" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A237" s="47">
@@ -21830,28 +21830,28 @@
       <c r="E342" s="49"/>
     </row>
     <row r="343" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A343" s="90">
+      <c r="A343" s="92">
         <v>5510105</v>
       </c>
-      <c r="B343" s="90" t="s">
+      <c r="B343" s="92" t="s">
         <v>954</v>
       </c>
-      <c r="C343" s="90">
+      <c r="C343" s="92">
         <v>6510105</v>
       </c>
       <c r="D343" s="69" t="s">
         <v>955</v>
       </c>
-      <c r="E343" s="92"/>
+      <c r="E343" s="99"/>
     </row>
     <row r="344" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A344" s="91"/>
-      <c r="B344" s="91"/>
-      <c r="C344" s="91"/>
+      <c r="A344" s="93"/>
+      <c r="B344" s="93"/>
+      <c r="C344" s="93"/>
       <c r="D344" s="48" t="s">
         <v>954</v>
       </c>
-      <c r="E344" s="93"/>
+      <c r="E344" s="100"/>
     </row>
     <row r="345" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A345" s="47">
@@ -22293,28 +22293,28 @@
       <c r="E377" s="49"/>
     </row>
     <row r="378" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A378" s="90">
+      <c r="A378" s="92">
         <v>5510215</v>
       </c>
-      <c r="B378" s="90" t="s">
+      <c r="B378" s="92" t="s">
         <v>986</v>
       </c>
-      <c r="C378" s="90">
+      <c r="C378" s="92">
         <v>6510215</v>
       </c>
       <c r="D378" s="69" t="s">
         <v>987</v>
       </c>
-      <c r="E378" s="92"/>
+      <c r="E378" s="99"/>
     </row>
     <row r="379" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A379" s="91"/>
-      <c r="B379" s="91"/>
-      <c r="C379" s="91"/>
+      <c r="A379" s="93"/>
+      <c r="B379" s="93"/>
+      <c r="C379" s="93"/>
       <c r="D379" s="48" t="s">
         <v>988</v>
       </c>
-      <c r="E379" s="93"/>
+      <c r="E379" s="100"/>
     </row>
     <row r="380" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A380" s="47">
@@ -22509,52 +22509,52 @@
       <c r="E395" s="49"/>
     </row>
     <row r="396" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A396" s="90">
+      <c r="A396" s="92">
         <v>5510312</v>
       </c>
-      <c r="B396" s="90" t="s">
+      <c r="B396" s="92" t="s">
         <v>1004</v>
       </c>
-      <c r="C396" s="90">
+      <c r="C396" s="92">
         <v>6510312</v>
       </c>
       <c r="D396" s="70" t="s">
         <v>1005</v>
       </c>
-      <c r="E396" s="92"/>
+      <c r="E396" s="99"/>
     </row>
     <row r="397" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A397" s="91"/>
-      <c r="B397" s="91"/>
-      <c r="C397" s="91"/>
+      <c r="A397" s="93"/>
+      <c r="B397" s="93"/>
+      <c r="C397" s="93"/>
       <c r="D397" s="48" t="s">
         <v>1006</v>
       </c>
-      <c r="E397" s="93"/>
+      <c r="E397" s="100"/>
     </row>
     <row r="398" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A398" s="90">
+      <c r="A398" s="92">
         <v>5510313</v>
       </c>
-      <c r="B398" s="94" t="s">
+      <c r="B398" s="101" t="s">
         <v>1007</v>
       </c>
-      <c r="C398" s="90">
+      <c r="C398" s="92">
         <v>6510313</v>
       </c>
       <c r="D398" s="70" t="s">
         <v>1008</v>
       </c>
-      <c r="E398" s="92"/>
+      <c r="E398" s="99"/>
     </row>
     <row r="399" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A399" s="91"/>
-      <c r="B399" s="95"/>
-      <c r="C399" s="91"/>
+      <c r="A399" s="93"/>
+      <c r="B399" s="102"/>
+      <c r="C399" s="93"/>
       <c r="D399" s="48" t="s">
         <v>1009</v>
       </c>
-      <c r="E399" s="93"/>
+      <c r="E399" s="100"/>
     </row>
     <row r="400" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A400" s="47">
@@ -22572,28 +22572,28 @@
       <c r="E400" s="49"/>
     </row>
     <row r="401" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A401" s="90">
+      <c r="A401" s="92">
         <v>5510315</v>
       </c>
-      <c r="B401" s="94" t="s">
+      <c r="B401" s="101" t="s">
         <v>1011</v>
       </c>
-      <c r="C401" s="90">
+      <c r="C401" s="92">
         <v>6510315</v>
       </c>
       <c r="D401" s="70" t="s">
         <v>1012</v>
       </c>
-      <c r="E401" s="92"/>
+      <c r="E401" s="99"/>
     </row>
     <row r="402" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A402" s="91"/>
-      <c r="B402" s="95"/>
-      <c r="C402" s="91"/>
+      <c r="A402" s="93"/>
+      <c r="B402" s="102"/>
+      <c r="C402" s="93"/>
       <c r="D402" s="48" t="s">
         <v>1013</v>
       </c>
-      <c r="E402" s="93"/>
+      <c r="E402" s="100"/>
     </row>
     <row r="403" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A403" s="40">
@@ -25356,28 +25356,28 @@
       <c r="E602" s="49"/>
     </row>
     <row r="603" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A603" s="90">
+      <c r="A603" s="92">
         <v>5520147</v>
       </c>
-      <c r="B603" s="90" t="s">
+      <c r="B603" s="92" t="s">
         <v>1205</v>
       </c>
-      <c r="C603" s="90">
+      <c r="C603" s="92">
         <v>6520147</v>
       </c>
       <c r="D603" s="69" t="s">
         <v>1206</v>
       </c>
-      <c r="E603" s="92"/>
+      <c r="E603" s="99"/>
     </row>
     <row r="604" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A604" s="91"/>
-      <c r="B604" s="91"/>
-      <c r="C604" s="91"/>
+      <c r="A604" s="93"/>
+      <c r="B604" s="93"/>
+      <c r="C604" s="93"/>
       <c r="D604" s="48" t="s">
         <v>1207</v>
       </c>
-      <c r="E604" s="93"/>
+      <c r="E604" s="100"/>
     </row>
     <row r="605" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A605" s="47">
@@ -25454,28 +25454,28 @@
       <c r="E610" s="49"/>
     </row>
     <row r="611" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A611" s="90">
+      <c r="A611" s="92">
         <v>5520154</v>
       </c>
-      <c r="B611" s="94" t="s">
+      <c r="B611" s="101" t="s">
         <v>1214</v>
       </c>
-      <c r="C611" s="90">
+      <c r="C611" s="92">
         <v>6520154</v>
       </c>
       <c r="D611" s="69" t="s">
         <v>1215</v>
       </c>
-      <c r="E611" s="92"/>
+      <c r="E611" s="99"/>
     </row>
     <row r="612" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A612" s="91"/>
-      <c r="B612" s="95"/>
-      <c r="C612" s="91"/>
+      <c r="A612" s="93"/>
+      <c r="B612" s="102"/>
+      <c r="C612" s="93"/>
       <c r="D612" s="48" t="s">
         <v>1216</v>
       </c>
-      <c r="E612" s="93"/>
+      <c r="E612" s="100"/>
     </row>
     <row r="613" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A613" s="47">
@@ -25857,25 +25857,25 @@
       <c r="E645" s="49"/>
     </row>
     <row r="646" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A646" s="90">
+      <c r="A646" s="92">
         <v>5520184</v>
       </c>
-      <c r="B646" s="90" t="s">
+      <c r="B646" s="92" t="s">
         <v>1246</v>
       </c>
-      <c r="C646" s="90">
+      <c r="C646" s="92">
         <v>6520184</v>
       </c>
-      <c r="D646" s="90" t="s">
+      <c r="D646" s="92" t="s">
         <v>1246</v>
       </c>
       <c r="E646" s="66"/>
     </row>
     <row r="647" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A647" s="91"/>
-      <c r="B647" s="91"/>
-      <c r="C647" s="91"/>
-      <c r="D647" s="91"/>
+      <c r="A647" s="93"/>
+      <c r="B647" s="93"/>
+      <c r="C647" s="93"/>
+      <c r="D647" s="93"/>
       <c r="E647" s="49"/>
     </row>
     <row r="648" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -26727,35 +26727,35 @@
       <c r="E709" s="49"/>
     </row>
     <row r="710" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A710" s="90">
+      <c r="A710" s="92">
         <v>5520243</v>
       </c>
-      <c r="B710" s="90" t="s">
+      <c r="B710" s="92" t="s">
         <v>1307</v>
       </c>
-      <c r="C710" s="90">
+      <c r="C710" s="92">
         <v>6520243</v>
       </c>
-      <c r="D710" s="90" t="s">
+      <c r="D710" s="92" t="s">
         <v>1307</v>
       </c>
       <c r="E710" s="66"/>
     </row>
     <row r="711" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A711" s="91"/>
-      <c r="B711" s="91"/>
-      <c r="C711" s="91"/>
-      <c r="D711" s="91"/>
+      <c r="A711" s="93"/>
+      <c r="B711" s="93"/>
+      <c r="C711" s="93"/>
+      <c r="D711" s="93"/>
       <c r="E711" s="49"/>
     </row>
     <row r="712" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A712" s="90">
+      <c r="A712" s="92">
         <v>5520244</v>
       </c>
-      <c r="B712" s="90" t="s">
+      <c r="B712" s="92" t="s">
         <v>1308</v>
       </c>
-      <c r="C712" s="90">
+      <c r="C712" s="92">
         <v>6520244</v>
       </c>
       <c r="D712" s="69" t="s">
@@ -26773,9 +26773,9 @@
       <c r="E713" s="66"/>
     </row>
     <row r="714" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A714" s="91"/>
-      <c r="B714" s="91"/>
-      <c r="C714" s="91"/>
+      <c r="A714" s="93"/>
+      <c r="B714" s="93"/>
+      <c r="C714" s="93"/>
       <c r="D714" s="74"/>
       <c r="E714" s="49"/>
     </row>
@@ -26888,25 +26888,25 @@
       <c r="E722" s="49"/>
     </row>
     <row r="723" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A723" s="90">
+      <c r="A723" s="92">
         <v>5520251</v>
       </c>
-      <c r="B723" s="90" t="s">
+      <c r="B723" s="92" t="s">
         <v>1317</v>
       </c>
-      <c r="C723" s="90">
+      <c r="C723" s="92">
         <v>6520251</v>
       </c>
-      <c r="D723" s="90" t="s">
+      <c r="D723" s="92" t="s">
         <v>1317</v>
       </c>
       <c r="E723" s="66"/>
     </row>
     <row r="724" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A724" s="91"/>
-      <c r="B724" s="91"/>
-      <c r="C724" s="91"/>
-      <c r="D724" s="91"/>
+      <c r="A724" s="93"/>
+      <c r="B724" s="93"/>
+      <c r="C724" s="93"/>
+      <c r="D724" s="93"/>
       <c r="E724" s="49"/>
     </row>
     <row r="725" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -28083,25 +28083,25 @@
       <c r="E811" s="49"/>
     </row>
     <row r="812" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A812" s="99">
+      <c r="A812" s="94">
         <v>55402</v>
       </c>
-      <c r="B812" s="99" t="s">
+      <c r="B812" s="94" t="s">
         <v>1399</v>
       </c>
-      <c r="C812" s="99">
+      <c r="C812" s="94">
         <v>65402</v>
       </c>
-      <c r="D812" s="99" t="s">
+      <c r="D812" s="94" t="s">
         <v>1399</v>
       </c>
       <c r="E812" s="75"/>
     </row>
     <row r="813" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A813" s="100"/>
-      <c r="B813" s="100"/>
-      <c r="C813" s="100"/>
-      <c r="D813" s="100"/>
+      <c r="A813" s="95"/>
+      <c r="B813" s="95"/>
+      <c r="C813" s="95"/>
+      <c r="D813" s="95"/>
       <c r="E813" s="42"/>
     </row>
     <row r="814" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -28584,10 +28584,10 @@
       <c r="E850" s="49"/>
     </row>
     <row r="851" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A851" s="90">
+      <c r="A851" s="92">
         <v>5580209</v>
       </c>
-      <c r="B851" s="90" t="s">
+      <c r="B851" s="92" t="s">
         <v>1433</v>
       </c>
       <c r="C851" s="96"/>
@@ -28595,8 +28595,8 @@
       <c r="E851" s="66"/>
     </row>
     <row r="852" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A852" s="91"/>
-      <c r="B852" s="91"/>
+      <c r="A852" s="93"/>
+      <c r="B852" s="93"/>
       <c r="C852" s="97"/>
       <c r="D852" s="97"/>
       <c r="E852" s="49"/>
@@ -28999,25 +28999,25 @@
       <c r="E883" s="49"/>
     </row>
     <row r="884" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A884" s="90">
+      <c r="A884" s="92">
         <v>5620123</v>
       </c>
-      <c r="B884" s="90" t="s">
+      <c r="B884" s="92" t="s">
         <v>1462</v>
       </c>
-      <c r="C884" s="90">
+      <c r="C884" s="92">
         <v>6620123</v>
       </c>
-      <c r="D884" s="90" t="s">
+      <c r="D884" s="92" t="s">
         <v>1462</v>
       </c>
       <c r="E884" s="66"/>
     </row>
     <row r="885" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A885" s="91"/>
-      <c r="B885" s="91"/>
-      <c r="C885" s="91"/>
-      <c r="D885" s="91"/>
+      <c r="A885" s="93"/>
+      <c r="B885" s="93"/>
+      <c r="C885" s="93"/>
+      <c r="D885" s="93"/>
       <c r="E885" s="49"/>
     </row>
     <row r="886" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -31197,28 +31197,28 @@
       <c r="E1045" s="49"/>
     </row>
     <row r="1046" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1046" s="99">
+      <c r="A1046" s="94">
         <v>58402</v>
       </c>
-      <c r="B1046" s="99" t="s">
+      <c r="B1046" s="94" t="s">
         <v>1611</v>
       </c>
-      <c r="C1046" s="99">
+      <c r="C1046" s="94">
         <v>68402</v>
       </c>
       <c r="D1046" s="69" t="s">
         <v>1612</v>
       </c>
-      <c r="E1046" s="101"/>
+      <c r="E1046" s="90"/>
     </row>
     <row r="1047" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1047" s="100"/>
-      <c r="B1047" s="100"/>
-      <c r="C1047" s="100"/>
+      <c r="A1047" s="95"/>
+      <c r="B1047" s="95"/>
+      <c r="C1047" s="95"/>
       <c r="D1047" s="41" t="s">
         <v>1611</v>
       </c>
-      <c r="E1047" s="102"/>
+      <c r="E1047" s="91"/>
     </row>
     <row r="1048" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1048" s="47">
@@ -32304,14 +32304,52 @@
     </row>
   </sheetData>
   <mergeCells count="69">
-    <mergeCell ref="E1046:E1047"/>
-    <mergeCell ref="A884:A885"/>
-    <mergeCell ref="B884:B885"/>
-    <mergeCell ref="C884:C885"/>
-    <mergeCell ref="D884:D885"/>
-    <mergeCell ref="A1046:A1047"/>
-    <mergeCell ref="B1046:B1047"/>
-    <mergeCell ref="C1046:C1047"/>
+    <mergeCell ref="A68:A69"/>
+    <mergeCell ref="B68:B69"/>
+    <mergeCell ref="C68:C69"/>
+    <mergeCell ref="D68:D69"/>
+    <mergeCell ref="A230:A231"/>
+    <mergeCell ref="C230:C231"/>
+    <mergeCell ref="E230:E231"/>
+    <mergeCell ref="A235:A236"/>
+    <mergeCell ref="C235:C236"/>
+    <mergeCell ref="E235:E236"/>
+    <mergeCell ref="A343:A344"/>
+    <mergeCell ref="B343:B344"/>
+    <mergeCell ref="C343:C344"/>
+    <mergeCell ref="E343:E344"/>
+    <mergeCell ref="A378:A379"/>
+    <mergeCell ref="B378:B379"/>
+    <mergeCell ref="C378:C379"/>
+    <mergeCell ref="E378:E379"/>
+    <mergeCell ref="A396:A397"/>
+    <mergeCell ref="B396:B397"/>
+    <mergeCell ref="C396:C397"/>
+    <mergeCell ref="E396:E397"/>
+    <mergeCell ref="A398:A399"/>
+    <mergeCell ref="B398:B399"/>
+    <mergeCell ref="C398:C399"/>
+    <mergeCell ref="E398:E399"/>
+    <mergeCell ref="A401:A402"/>
+    <mergeCell ref="B401:B402"/>
+    <mergeCell ref="C401:C402"/>
+    <mergeCell ref="E401:E402"/>
+    <mergeCell ref="A603:A604"/>
+    <mergeCell ref="B603:B604"/>
+    <mergeCell ref="C603:C604"/>
+    <mergeCell ref="E603:E604"/>
+    <mergeCell ref="A611:A612"/>
+    <mergeCell ref="B611:B612"/>
+    <mergeCell ref="C611:C612"/>
+    <mergeCell ref="E611:E612"/>
+    <mergeCell ref="A646:A647"/>
+    <mergeCell ref="B646:B647"/>
+    <mergeCell ref="C646:C647"/>
+    <mergeCell ref="D646:D647"/>
+    <mergeCell ref="A710:A711"/>
+    <mergeCell ref="B710:B711"/>
+    <mergeCell ref="C710:C711"/>
+    <mergeCell ref="D710:D711"/>
     <mergeCell ref="A851:A852"/>
     <mergeCell ref="B851:B852"/>
     <mergeCell ref="C851:C852"/>
@@ -32327,52 +32365,14 @@
     <mergeCell ref="B812:B813"/>
     <mergeCell ref="C812:C813"/>
     <mergeCell ref="D812:D813"/>
-    <mergeCell ref="A646:A647"/>
-    <mergeCell ref="B646:B647"/>
-    <mergeCell ref="C646:C647"/>
-    <mergeCell ref="D646:D647"/>
-    <mergeCell ref="A710:A711"/>
-    <mergeCell ref="B710:B711"/>
-    <mergeCell ref="C710:C711"/>
-    <mergeCell ref="D710:D711"/>
-    <mergeCell ref="A603:A604"/>
-    <mergeCell ref="B603:B604"/>
-    <mergeCell ref="C603:C604"/>
-    <mergeCell ref="E603:E604"/>
-    <mergeCell ref="A611:A612"/>
-    <mergeCell ref="B611:B612"/>
-    <mergeCell ref="C611:C612"/>
-    <mergeCell ref="E611:E612"/>
-    <mergeCell ref="A398:A399"/>
-    <mergeCell ref="B398:B399"/>
-    <mergeCell ref="C398:C399"/>
-    <mergeCell ref="E398:E399"/>
-    <mergeCell ref="A401:A402"/>
-    <mergeCell ref="B401:B402"/>
-    <mergeCell ref="C401:C402"/>
-    <mergeCell ref="E401:E402"/>
-    <mergeCell ref="A378:A379"/>
-    <mergeCell ref="B378:B379"/>
-    <mergeCell ref="C378:C379"/>
-    <mergeCell ref="E378:E379"/>
-    <mergeCell ref="A396:A397"/>
-    <mergeCell ref="B396:B397"/>
-    <mergeCell ref="C396:C397"/>
-    <mergeCell ref="E396:E397"/>
-    <mergeCell ref="E230:E231"/>
-    <mergeCell ref="A235:A236"/>
-    <mergeCell ref="C235:C236"/>
-    <mergeCell ref="E235:E236"/>
-    <mergeCell ref="A343:A344"/>
-    <mergeCell ref="B343:B344"/>
-    <mergeCell ref="C343:C344"/>
-    <mergeCell ref="E343:E344"/>
-    <mergeCell ref="A68:A69"/>
-    <mergeCell ref="B68:B69"/>
-    <mergeCell ref="C68:C69"/>
-    <mergeCell ref="D68:D69"/>
-    <mergeCell ref="A230:A231"/>
-    <mergeCell ref="C230:C231"/>
+    <mergeCell ref="E1046:E1047"/>
+    <mergeCell ref="A884:A885"/>
+    <mergeCell ref="B884:B885"/>
+    <mergeCell ref="C884:C885"/>
+    <mergeCell ref="D884:D885"/>
+    <mergeCell ref="A1046:A1047"/>
+    <mergeCell ref="B1046:B1047"/>
+    <mergeCell ref="C1046:C1047"/>
   </mergeCells>
   <conditionalFormatting sqref="G4:H9">
     <cfRule type="duplicateValues" dxfId="7" priority="8"/>

</xml_diff>

<commit_message>
Update DS_LOP_(Mau).xlsx with new data
</commit_message>
<xml_diff>
--- a/data_base/DS_LOP_(Mau).xlsx
+++ b/data_base/DS_LOP_(Mau).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sumik\Downloads\ke-khai-gio-day-app-master\data_base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69511399-58BC-4D8D-ACE0-4F3EAB9ED70F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0952A1D-4E93-46AD-8278-9AC1D582D1CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9BE4D872-0846-4818-A986-007578B8C884}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{9BE4D872-0846-4818-A986-007578B8C884}"/>
   </bookViews>
   <sheets>
     <sheet name="DANH_MUC" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4536" uniqueCount="1733">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4684" uniqueCount="1748">
   <si>
     <t>Khoá học</t>
   </si>
@@ -5239,6 +5239,51 @@
   </si>
   <si>
     <t>110</t>
+  </si>
+  <si>
+    <t>CĐ_CHẾ BIẾN MÓN ĂN</t>
+  </si>
+  <si>
+    <t>TC_CÔNG NGHỆ KỸ THUẬT ĐIỆN, ĐIỆN TỬ</t>
+  </si>
+  <si>
+    <t>MON224Z</t>
+  </si>
+  <si>
+    <t>MON110Z</t>
+  </si>
+  <si>
+    <t>Thương phẩm an toàn thực phẩm</t>
+  </si>
+  <si>
+    <t>Tổng quan du lịch và khách sạn</t>
+  </si>
+  <si>
+    <t>Môi trường và an ninh - an toàn trong du lịch</t>
+  </si>
+  <si>
+    <t>Tâm lý và kỹ năng giao tiếp với khách du lịch</t>
+  </si>
+  <si>
+    <t>Kỹ thuật trang trí bánh kem</t>
+  </si>
+  <si>
+    <t>Kỹ thuật Pha chế đồ uống</t>
+  </si>
+  <si>
+    <t>Nghiệp vụ nhà hàng</t>
+  </si>
+  <si>
+    <t>Kỹ thuật cắt thái và tỉa hoa trang trí</t>
+  </si>
+  <si>
+    <t>Chế biến món ăn Việt Nam</t>
+  </si>
+  <si>
+    <t>Chế biến món ăn Á</t>
+  </si>
+  <si>
+    <t>Chế biến món ăn Âu</t>
   </si>
 </sst>
 </file>
@@ -5720,7 +5765,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -5967,31 +6012,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -6006,12 +6030,157 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Excel Built-in Normal" xfId="1" xr:uid="{D165A2DC-E562-4944-81AC-765134482C48}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="21">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -6381,7 +6550,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:L122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="C40" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
@@ -9091,10 +9260,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB7FB4C3-C8C2-44EC-BC34-2B5E4447113E}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:BM1129"/>
+  <dimension ref="A1:BQ1129"/>
   <sheetViews>
-    <sheetView topLeftCell="AQ1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="BC14" sqref="BC14"/>
+    <sheetView tabSelected="1" topLeftCell="BE1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BQ3" sqref="BQ3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -9163,10 +9332,14 @@
     <col min="63" max="63" width="21.21875" style="43" customWidth="1"/>
     <col min="64" max="64" width="5.21875" style="43" customWidth="1"/>
     <col min="65" max="65" width="21" style="43" customWidth="1"/>
-    <col min="66" max="16384" width="8.88671875" style="22"/>
+    <col min="66" max="66" width="5.21875" style="112" customWidth="1"/>
+    <col min="67" max="67" width="21" style="43" customWidth="1"/>
+    <col min="68" max="68" width="5.21875" style="112" customWidth="1"/>
+    <col min="69" max="69" width="21" style="43" customWidth="1"/>
+    <col min="70" max="16384" width="8.88671875" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:65" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:69" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
         <v>145</v>
       </c>
@@ -9357,8 +9530,20 @@
       <c r="BM1" s="25" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="2" spans="1:65" s="29" customFormat="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="BN1" s="25" t="s">
+        <v>150</v>
+      </c>
+      <c r="BO1" s="25" t="s">
+        <v>1733</v>
+      </c>
+      <c r="BP1" s="25" t="s">
+        <v>150</v>
+      </c>
+      <c r="BQ1" s="25" t="s">
+        <v>1734</v>
+      </c>
+    </row>
+    <row r="2" spans="1:69" s="29" customFormat="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="26">
         <v>5</v>
       </c>
@@ -9491,8 +9676,16 @@
       <c r="BM2" s="24" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="3" spans="1:65" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BN2" s="31"/>
+      <c r="BO2" s="24" t="s">
+        <v>1736</v>
+      </c>
+      <c r="BP2" s="31"/>
+      <c r="BQ2" s="24" t="s">
+        <v>1735</v>
+      </c>
+    </row>
+    <row r="3" spans="1:69" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="33">
         <v>514</v>
       </c>
@@ -9681,8 +9874,20 @@
       <c r="BM3" s="38" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="4" spans="1:65" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BN3" s="107" t="s">
+        <v>214</v>
+      </c>
+      <c r="BO3" s="38" t="s">
+        <v>213</v>
+      </c>
+      <c r="BP3" s="107" t="s">
+        <v>214</v>
+      </c>
+      <c r="BQ3" s="38" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="4" spans="1:69" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="40">
         <v>51402</v>
       </c>
@@ -9871,8 +10076,20 @@
       <c r="BM4" s="45" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="5" spans="1:65" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BN4" s="108" t="s">
+        <v>219</v>
+      </c>
+      <c r="BO4" s="45" t="s">
+        <v>218</v>
+      </c>
+      <c r="BP4" s="107" t="s">
+        <v>219</v>
+      </c>
+      <c r="BQ4" s="45" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="5" spans="1:69" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="47">
         <v>5140201</v>
       </c>
@@ -10061,8 +10278,20 @@
       <c r="BM5" s="45" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="6" spans="1:65" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BN5" s="108" t="s">
+        <v>223</v>
+      </c>
+      <c r="BO5" s="45" t="s">
+        <v>222</v>
+      </c>
+      <c r="BP5" s="107" t="s">
+        <v>223</v>
+      </c>
+      <c r="BQ5" s="45" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="6" spans="1:69" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="51"/>
       <c r="B6" s="52"/>
       <c r="C6" s="48">
@@ -10247,8 +10476,20 @@
       <c r="BM6" s="45" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="7" spans="1:65" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BN6" s="108" t="s">
+        <v>227</v>
+      </c>
+      <c r="BO6" s="45" t="s">
+        <v>226</v>
+      </c>
+      <c r="BP6" s="107" t="s">
+        <v>227</v>
+      </c>
+      <c r="BQ6" s="45" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="7" spans="1:69" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="51"/>
       <c r="B7" s="52"/>
       <c r="C7" s="48">
@@ -10433,8 +10674,20 @@
       <c r="BM7" s="45" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="8" spans="1:65" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BN7" s="108" t="s">
+        <v>234</v>
+      </c>
+      <c r="BO7" s="45" t="s">
+        <v>233</v>
+      </c>
+      <c r="BP7" s="107" t="s">
+        <v>234</v>
+      </c>
+      <c r="BQ7" s="45" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="8" spans="1:69" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="47">
         <v>5140204</v>
       </c>
@@ -10623,8 +10876,20 @@
       <c r="BM8" s="45" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="9" spans="1:65" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BN8" s="108" t="s">
+        <v>238</v>
+      </c>
+      <c r="BO8" s="45" t="s">
+        <v>239</v>
+      </c>
+      <c r="BP8" s="107" t="s">
+        <v>238</v>
+      </c>
+      <c r="BQ8" s="45" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="9" spans="1:69" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="51"/>
       <c r="B9" s="52"/>
       <c r="C9" s="48">
@@ -10809,8 +11074,20 @@
       <c r="BM9" s="45" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="10" spans="1:65" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BN9" s="108" t="s">
+        <v>245</v>
+      </c>
+      <c r="BO9" s="45" t="s">
+        <v>244</v>
+      </c>
+      <c r="BP9" s="107" t="s">
+        <v>247</v>
+      </c>
+      <c r="BQ9" s="45" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="10" spans="1:69" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="33">
         <v>521</v>
       </c>
@@ -10999,8 +11276,20 @@
       <c r="BM10" s="45" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="11" spans="1:65" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BN10" s="108" t="s">
+        <v>240</v>
+      </c>
+      <c r="BO10" s="45" t="s">
+        <v>241</v>
+      </c>
+      <c r="BP10" s="107" t="s">
+        <v>240</v>
+      </c>
+      <c r="BQ10" s="45" t="s">
+        <v>1737</v>
+      </c>
+    </row>
+    <row r="11" spans="1:69" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="40">
         <v>52101</v>
       </c>
@@ -11189,8 +11478,20 @@
       <c r="BM11" s="45" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="12" spans="1:65" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BN11" s="108" t="s">
+        <v>271</v>
+      </c>
+      <c r="BO11" s="45" t="s">
+        <v>274</v>
+      </c>
+      <c r="BP11" s="107" t="s">
+        <v>271</v>
+      </c>
+      <c r="BQ11" s="45" t="s">
+        <v>1738</v>
+      </c>
+    </row>
+    <row r="12" spans="1:69" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="47">
         <v>5210101</v>
       </c>
@@ -11379,8 +11680,20 @@
       <c r="BM12" s="45" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="13" spans="1:65" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BN12" s="108" t="s">
+        <v>250</v>
+      </c>
+      <c r="BO12" s="45" t="s">
+        <v>292</v>
+      </c>
+      <c r="BP12" s="107" t="s">
+        <v>250</v>
+      </c>
+      <c r="BQ12" s="45" t="s">
+        <v>1739</v>
+      </c>
+    </row>
+    <row r="13" spans="1:69" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="47">
         <v>5210102</v>
       </c>
@@ -11569,8 +11882,20 @@
       <c r="BM13" s="45" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="14" spans="1:65" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BN13" s="108" t="s">
+        <v>308</v>
+      </c>
+      <c r="BO13" s="45" t="s">
+        <v>309</v>
+      </c>
+      <c r="BP13" s="107" t="s">
+        <v>308</v>
+      </c>
+      <c r="BQ13" s="45" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="14" spans="1:69" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="47">
         <v>5210103</v>
       </c>
@@ -11759,8 +12084,20 @@
       <c r="BM14" s="45" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="15" spans="1:65" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BN14" s="108" t="s">
+        <v>284</v>
+      </c>
+      <c r="BO14" s="45" t="s">
+        <v>328</v>
+      </c>
+      <c r="BP14" s="107" t="s">
+        <v>284</v>
+      </c>
+      <c r="BQ14" s="45" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="15" spans="1:69" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="47">
         <v>5210104</v>
       </c>
@@ -11947,8 +12284,20 @@
       <c r="BM15" s="45" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="16" spans="1:65" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BN15" s="108" t="s">
+        <v>347</v>
+      </c>
+      <c r="BO15" s="45" t="s">
+        <v>349</v>
+      </c>
+      <c r="BP15" s="107" t="s">
+        <v>346</v>
+      </c>
+      <c r="BQ15" s="45" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="16" spans="1:69" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="47">
         <v>5210105</v>
       </c>
@@ -12137,8 +12486,20 @@
       <c r="BM16" s="45" t="s">
         <v>382</v>
       </c>
-    </row>
-    <row r="17" spans="1:65" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BN16" s="108" t="s">
+        <v>364</v>
+      </c>
+      <c r="BO16" s="45" t="s">
+        <v>294</v>
+      </c>
+      <c r="BP16" s="107" t="s">
+        <v>373</v>
+      </c>
+      <c r="BQ16" s="45" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="17" spans="1:69" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="40">
         <v>52102</v>
       </c>
@@ -12327,8 +12688,20 @@
       <c r="BM17" s="45" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="18" spans="1:65" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BN17" s="108" t="s">
+        <v>390</v>
+      </c>
+      <c r="BO17" s="45" t="s">
+        <v>389</v>
+      </c>
+      <c r="BP17" s="107" t="s">
+        <v>386</v>
+      </c>
+      <c r="BQ17" s="45" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="18" spans="1:69" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="47">
         <v>5210201</v>
       </c>
@@ -12513,8 +12886,20 @@
       <c r="BM18" s="45" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="19" spans="1:65" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BN18" s="108" t="s">
+        <v>410</v>
+      </c>
+      <c r="BO18" s="45" t="s">
+        <v>277</v>
+      </c>
+      <c r="BP18" s="107" t="s">
+        <v>410</v>
+      </c>
+      <c r="BQ18" s="45" t="s">
+        <v>1740</v>
+      </c>
+    </row>
+    <row r="19" spans="1:69" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="47">
         <v>5210202</v>
       </c>
@@ -12703,8 +13088,20 @@
       <c r="BM19" s="45" t="s">
         <v>376</v>
       </c>
-    </row>
-    <row r="20" spans="1:65" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BN19" s="108" t="s">
+        <v>358</v>
+      </c>
+      <c r="BO19" s="45" t="s">
+        <v>391</v>
+      </c>
+      <c r="BP19" s="107" t="s">
+        <v>440</v>
+      </c>
+      <c r="BQ19" s="45" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="20" spans="1:69" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="47">
         <v>5210203</v>
       </c>
@@ -12889,8 +13286,20 @@
       <c r="BM20" s="45" t="s">
         <v>474</v>
       </c>
-    </row>
-    <row r="21" spans="1:65" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BN20" s="108" t="s">
+        <v>378</v>
+      </c>
+      <c r="BO20" s="45" t="s">
+        <v>435</v>
+      </c>
+      <c r="BP20" s="107" t="s">
+        <v>378</v>
+      </c>
+      <c r="BQ20" s="45" t="s">
+        <v>1744</v>
+      </c>
+    </row>
+    <row r="21" spans="1:69" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="47">
         <v>5210204</v>
       </c>
@@ -13075,8 +13484,20 @@
       <c r="BM21" s="45" t="s">
         <v>423</v>
       </c>
-    </row>
-    <row r="22" spans="1:65" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BN21" s="108" t="s">
+        <v>401</v>
+      </c>
+      <c r="BO21" s="45" t="s">
+        <v>540</v>
+      </c>
+      <c r="BP21" s="107" t="s">
+        <v>401</v>
+      </c>
+      <c r="BQ21" s="45" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="22" spans="1:69" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="47">
         <v>5210205</v>
       </c>
@@ -13261,8 +13682,20 @@
       <c r="BM22" s="45" t="s">
         <v>510</v>
       </c>
-    </row>
-    <row r="23" spans="1:65" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BN22" s="108" t="s">
+        <v>425</v>
+      </c>
+      <c r="BO22" s="45" t="s">
+        <v>437</v>
+      </c>
+      <c r="BP22" s="107" t="s">
+        <v>425</v>
+      </c>
+      <c r="BQ22" s="45" t="s">
+        <v>1745</v>
+      </c>
+    </row>
+    <row r="23" spans="1:69" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="47">
         <v>5210206</v>
       </c>
@@ -13447,8 +13880,20 @@
       <c r="BM23" s="45" t="s">
         <v>543</v>
       </c>
-    </row>
-    <row r="24" spans="1:65" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BN23" s="103" t="s">
+        <v>530</v>
+      </c>
+      <c r="BO23" s="104" t="s">
+        <v>286</v>
+      </c>
+      <c r="BP23" s="113" t="s">
+        <v>509</v>
+      </c>
+      <c r="BQ23" s="104" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="24" spans="1:69" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="47">
         <v>5210207</v>
       </c>
@@ -13633,8 +14078,20 @@
       <c r="BM24" s="45" t="s">
         <v>563</v>
       </c>
-    </row>
-    <row r="25" spans="1:65" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BN24" s="103" t="s">
+        <v>541</v>
+      </c>
+      <c r="BO24" s="104" t="s">
+        <v>460</v>
+      </c>
+      <c r="BP24" s="113" t="s">
+        <v>541</v>
+      </c>
+      <c r="BQ24" s="105" t="s">
+        <v>1746</v>
+      </c>
+    </row>
+    <row r="25" spans="1:69" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="47">
         <v>5210208</v>
       </c>
@@ -13817,8 +14274,20 @@
       <c r="BM25" s="45" t="s">
         <v>582</v>
       </c>
-    </row>
-    <row r="26" spans="1:65" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BN25" s="109" t="s">
+        <v>561</v>
+      </c>
+      <c r="BO25" s="105" t="s">
+        <v>568</v>
+      </c>
+      <c r="BP25" s="113" t="s">
+        <v>561</v>
+      </c>
+      <c r="BQ25" s="105" t="s">
+        <v>1747</v>
+      </c>
+    </row>
+    <row r="26" spans="1:69" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="57"/>
       <c r="G26" s="43"/>
       <c r="H26" s="53"/>
@@ -13983,8 +14452,20 @@
       <c r="BM26" s="45" t="s">
         <v>489</v>
       </c>
-    </row>
-    <row r="27" spans="1:65" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BN26" s="109" t="s">
+        <v>580</v>
+      </c>
+      <c r="BO26" s="105" t="s">
+        <v>632</v>
+      </c>
+      <c r="BP26" s="113" t="s">
+        <v>580</v>
+      </c>
+      <c r="BQ26" s="104" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="27" spans="1:69" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="60" t="s">
         <v>145</v>
       </c>
@@ -14157,8 +14638,20 @@
       <c r="BM27" s="45" t="s">
         <v>535</v>
       </c>
-    </row>
-    <row r="28" spans="1:65" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BN27" s="106" t="s">
+        <v>520</v>
+      </c>
+      <c r="BO27" s="104" t="s">
+        <v>588</v>
+      </c>
+      <c r="BP27" s="113" t="s">
+        <v>520</v>
+      </c>
+      <c r="BQ27" s="104" t="s">
+        <v>1741</v>
+      </c>
+    </row>
+    <row r="28" spans="1:69" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="47">
         <v>5210209</v>
       </c>
@@ -14307,8 +14800,20 @@
       <c r="BM28" s="62" t="s">
         <v>557</v>
       </c>
-    </row>
-    <row r="29" spans="1:65" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BN28" s="106" t="s">
+        <v>150</v>
+      </c>
+      <c r="BO28" s="104" t="s">
+        <v>150</v>
+      </c>
+      <c r="BP28" s="113" t="s">
+        <v>583</v>
+      </c>
+      <c r="BQ28" s="105" t="s">
+        <v>1742</v>
+      </c>
+    </row>
+    <row r="29" spans="1:69" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="47">
         <v>5210210</v>
       </c>
@@ -14441,8 +14946,16 @@
       <c r="BM29" s="62" t="s">
         <v>575</v>
       </c>
-    </row>
-    <row r="30" spans="1:65" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BN29" s="109"/>
+      <c r="BO29" s="105"/>
+      <c r="BP29" s="113" t="s">
+        <v>597</v>
+      </c>
+      <c r="BQ29" s="105" t="s">
+        <v>1743</v>
+      </c>
+    </row>
+    <row r="30" spans="1:69" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="47">
         <v>5210211</v>
       </c>
@@ -14555,8 +15068,16 @@
       <c r="BM30" s="56" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="31" spans="1:65" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BN30" s="109"/>
+      <c r="BO30" s="105"/>
+      <c r="BP30" s="113" t="s">
+        <v>616</v>
+      </c>
+      <c r="BQ30" s="105" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="31" spans="1:69" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="51"/>
       <c r="B31" s="52"/>
       <c r="C31" s="48">
@@ -14667,8 +15188,16 @@
       <c r="BM31" s="56" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="32" spans="1:65" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BN31" s="109"/>
+      <c r="BO31" s="105"/>
+      <c r="BP31" s="113" t="s">
+        <v>623</v>
+      </c>
+      <c r="BQ31" s="105" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="32" spans="1:69" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="47">
         <v>5210213</v>
       </c>
@@ -14777,8 +15306,16 @@
       <c r="BK32" s="62"/>
       <c r="BL32" s="62"/>
       <c r="BM32" s="62"/>
-    </row>
-    <row r="33" spans="1:65" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BN32" s="109"/>
+      <c r="BO32" s="105"/>
+      <c r="BP32" s="113" t="s">
+        <v>628</v>
+      </c>
+      <c r="BQ32" s="105" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="33" spans="1:69" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="47">
         <v>5210214</v>
       </c>
@@ -14953,8 +15490,20 @@
       <c r="BK33" s="62"/>
       <c r="BL33" s="62"/>
       <c r="BM33" s="62"/>
-    </row>
-    <row r="34" spans="1:65" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BN33" s="110" t="s">
+        <v>150</v>
+      </c>
+      <c r="BO33" s="62" t="s">
+        <v>150</v>
+      </c>
+      <c r="BP33" s="110" t="s">
+        <v>150</v>
+      </c>
+      <c r="BQ33" s="62" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="34" spans="1:69" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="51"/>
       <c r="B34" s="52"/>
       <c r="C34" s="48">
@@ -15125,8 +15674,20 @@
       <c r="BK34" s="62"/>
       <c r="BL34" s="62"/>
       <c r="BM34" s="62"/>
-    </row>
-    <row r="35" spans="1:65" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BN34" s="110" t="s">
+        <v>150</v>
+      </c>
+      <c r="BO34" s="62" t="s">
+        <v>150</v>
+      </c>
+      <c r="BP34" s="110" t="s">
+        <v>150</v>
+      </c>
+      <c r="BQ34" s="62" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="35" spans="1:69" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="47">
         <v>5210216</v>
       </c>
@@ -15297,8 +15858,20 @@
       <c r="BK35" s="62"/>
       <c r="BL35" s="62"/>
       <c r="BM35" s="62"/>
-    </row>
-    <row r="36" spans="1:65" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BN35" s="110" t="s">
+        <v>150</v>
+      </c>
+      <c r="BO35" s="62" t="s">
+        <v>150</v>
+      </c>
+      <c r="BP35" s="110" t="s">
+        <v>150</v>
+      </c>
+      <c r="BQ35" s="62" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="36" spans="1:69" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="47">
         <v>5210217</v>
       </c>
@@ -15481,8 +16054,20 @@
       <c r="BM36" s="62" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="37" spans="1:65" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BN36" s="110" t="s">
+        <v>150</v>
+      </c>
+      <c r="BO36" s="62" t="s">
+        <v>150</v>
+      </c>
+      <c r="BP36" s="110" t="s">
+        <v>150</v>
+      </c>
+      <c r="BQ36" s="62" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="37" spans="1:69" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="47">
         <v>5210218</v>
       </c>
@@ -15665,8 +16250,20 @@
       <c r="BM37" s="62" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="38" spans="1:65" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BN37" s="110" t="s">
+        <v>150</v>
+      </c>
+      <c r="BO37" s="62" t="s">
+        <v>150</v>
+      </c>
+      <c r="BP37" s="110" t="s">
+        <v>150</v>
+      </c>
+      <c r="BQ37" s="62" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="38" spans="1:69" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="47">
         <v>5210219</v>
       </c>
@@ -15849,8 +16446,20 @@
       <c r="BM38" s="62" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="39" spans="1:65" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BN38" s="110" t="s">
+        <v>150</v>
+      </c>
+      <c r="BO38" s="62" t="s">
+        <v>150</v>
+      </c>
+      <c r="BP38" s="110" t="s">
+        <v>150</v>
+      </c>
+      <c r="BQ38" s="62" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="39" spans="1:69" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="47">
         <v>5210220</v>
       </c>
@@ -16033,8 +16642,20 @@
       <c r="BM39" s="62" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="40" spans="1:65" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BN39" s="110" t="s">
+        <v>150</v>
+      </c>
+      <c r="BO39" s="62" t="s">
+        <v>150</v>
+      </c>
+      <c r="BP39" s="110" t="s">
+        <v>150</v>
+      </c>
+      <c r="BQ39" s="62" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="40" spans="1:69" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="47">
         <v>5210221</v>
       </c>
@@ -16221,8 +16842,16 @@
       <c r="BM40" s="62" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="41" spans="1:65" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BN40" s="110" t="s">
+        <v>150</v>
+      </c>
+      <c r="BO40" s="62" t="s">
+        <v>150</v>
+      </c>
+      <c r="BP40" s="59"/>
+      <c r="BQ40" s="63"/>
+    </row>
+    <row r="41" spans="1:69" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="47">
         <v>5210222</v>
       </c>
@@ -16409,8 +17038,12 @@
       <c r="BM41" s="62" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="42" spans="1:65" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BN41" s="59"/>
+      <c r="BO41" s="63"/>
+      <c r="BP41" s="111"/>
+      <c r="BQ41" s="65"/>
+    </row>
+    <row r="42" spans="1:69" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="47">
         <v>5210223</v>
       </c>
@@ -16593,8 +17226,10 @@
       <c r="BM42" s="62" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="43" spans="1:65" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BN42" s="111"/>
+      <c r="BO42" s="65"/>
+    </row>
+    <row r="43" spans="1:69" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="47">
         <v>5210224</v>
       </c>
@@ -16778,7 +17413,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="44" spans="1:65" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:69" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="47">
         <v>5210225</v>
       </c>
@@ -16852,7 +17487,7 @@
       <c r="BL44" s="63"/>
       <c r="BM44" s="63"/>
     </row>
-    <row r="45" spans="1:65" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:69" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="47">
         <v>5210226</v>
       </c>
@@ -16922,7 +17557,7 @@
       <c r="BL45" s="65"/>
       <c r="BM45" s="65"/>
     </row>
-    <row r="46" spans="1:65" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:69" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="47">
         <v>5210227</v>
       </c>
@@ -16939,7 +17574,7 @@
       <c r="G46" s="43"/>
       <c r="H46" s="65"/>
     </row>
-    <row r="47" spans="1:65" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:69" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="47">
         <v>5210228</v>
       </c>
@@ -16956,7 +17591,7 @@
       <c r="G47" s="43"/>
       <c r="H47" s="43"/>
     </row>
-    <row r="48" spans="1:65" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:69" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="47">
         <v>5210229</v>
       </c>
@@ -17245,25 +17880,25 @@
       <c r="E67" s="49"/>
     </row>
     <row r="68" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="92">
+      <c r="A68" s="90">
         <v>5210305</v>
       </c>
-      <c r="B68" s="92" t="s">
+      <c r="B68" s="90" t="s">
         <v>689</v>
       </c>
-      <c r="C68" s="92">
+      <c r="C68" s="90">
         <v>6210305</v>
       </c>
-      <c r="D68" s="92" t="s">
+      <c r="D68" s="90" t="s">
         <v>689</v>
       </c>
       <c r="E68" s="66"/>
     </row>
     <row r="69" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="93"/>
-      <c r="B69" s="93"/>
-      <c r="C69" s="93"/>
-      <c r="D69" s="93"/>
+      <c r="A69" s="91"/>
+      <c r="B69" s="91"/>
+      <c r="C69" s="91"/>
+      <c r="D69" s="91"/>
       <c r="E69" s="49"/>
     </row>
     <row r="70" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -20259,30 +20894,30 @@
       <c r="E229" s="49"/>
     </row>
     <row r="230" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A230" s="92">
+      <c r="A230" s="90">
         <v>5340410</v>
       </c>
       <c r="B230" s="69" t="s">
         <v>849</v>
       </c>
-      <c r="C230" s="92">
+      <c r="C230" s="90">
         <v>6340410</v>
       </c>
       <c r="D230" s="70" t="s">
         <v>849</v>
       </c>
-      <c r="E230" s="99"/>
+      <c r="E230" s="92"/>
     </row>
     <row r="231" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A231" s="93"/>
+      <c r="A231" s="91"/>
       <c r="B231" s="48" t="s">
         <v>850</v>
       </c>
-      <c r="C231" s="93"/>
+      <c r="C231" s="91"/>
       <c r="D231" s="48" t="s">
         <v>850</v>
       </c>
-      <c r="E231" s="100"/>
+      <c r="E231" s="93"/>
     </row>
     <row r="232" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A232" s="47">
@@ -20330,30 +20965,30 @@
       <c r="E234" s="49"/>
     </row>
     <row r="235" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A235" s="92">
+      <c r="A235" s="90">
         <v>5340414</v>
       </c>
       <c r="B235" s="69" t="s">
         <v>856</v>
       </c>
-      <c r="C235" s="92">
+      <c r="C235" s="90">
         <v>6340414</v>
       </c>
       <c r="D235" s="70" t="s">
         <v>856</v>
       </c>
-      <c r="E235" s="99"/>
+      <c r="E235" s="92"/>
     </row>
     <row r="236" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A236" s="93"/>
+      <c r="A236" s="91"/>
       <c r="B236" s="48" t="s">
         <v>857</v>
       </c>
-      <c r="C236" s="93"/>
+      <c r="C236" s="91"/>
       <c r="D236" s="48" t="s">
         <v>857</v>
       </c>
-      <c r="E236" s="100"/>
+      <c r="E236" s="93"/>
     </row>
     <row r="237" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A237" s="47">
@@ -21830,28 +22465,28 @@
       <c r="E342" s="49"/>
     </row>
     <row r="343" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A343" s="92">
+      <c r="A343" s="90">
         <v>5510105</v>
       </c>
-      <c r="B343" s="92" t="s">
+      <c r="B343" s="90" t="s">
         <v>954</v>
       </c>
-      <c r="C343" s="92">
+      <c r="C343" s="90">
         <v>6510105</v>
       </c>
       <c r="D343" s="69" t="s">
         <v>955</v>
       </c>
-      <c r="E343" s="99"/>
+      <c r="E343" s="92"/>
     </row>
     <row r="344" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A344" s="93"/>
-      <c r="B344" s="93"/>
-      <c r="C344" s="93"/>
+      <c r="A344" s="91"/>
+      <c r="B344" s="91"/>
+      <c r="C344" s="91"/>
       <c r="D344" s="48" t="s">
         <v>954</v>
       </c>
-      <c r="E344" s="100"/>
+      <c r="E344" s="93"/>
     </row>
     <row r="345" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A345" s="47">
@@ -22293,28 +22928,28 @@
       <c r="E377" s="49"/>
     </row>
     <row r="378" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A378" s="92">
+      <c r="A378" s="90">
         <v>5510215</v>
       </c>
-      <c r="B378" s="92" t="s">
+      <c r="B378" s="90" t="s">
         <v>986</v>
       </c>
-      <c r="C378" s="92">
+      <c r="C378" s="90">
         <v>6510215</v>
       </c>
       <c r="D378" s="69" t="s">
         <v>987</v>
       </c>
-      <c r="E378" s="99"/>
+      <c r="E378" s="92"/>
     </row>
     <row r="379" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A379" s="93"/>
-      <c r="B379" s="93"/>
-      <c r="C379" s="93"/>
+      <c r="A379" s="91"/>
+      <c r="B379" s="91"/>
+      <c r="C379" s="91"/>
       <c r="D379" s="48" t="s">
         <v>988</v>
       </c>
-      <c r="E379" s="100"/>
+      <c r="E379" s="93"/>
     </row>
     <row r="380" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A380" s="47">
@@ -22509,52 +23144,52 @@
       <c r="E395" s="49"/>
     </row>
     <row r="396" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A396" s="92">
+      <c r="A396" s="90">
         <v>5510312</v>
       </c>
-      <c r="B396" s="92" t="s">
+      <c r="B396" s="90" t="s">
         <v>1004</v>
       </c>
-      <c r="C396" s="92">
+      <c r="C396" s="90">
         <v>6510312</v>
       </c>
       <c r="D396" s="70" t="s">
         <v>1005</v>
       </c>
-      <c r="E396" s="99"/>
+      <c r="E396" s="92"/>
     </row>
     <row r="397" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A397" s="93"/>
-      <c r="B397" s="93"/>
-      <c r="C397" s="93"/>
+      <c r="A397" s="91"/>
+      <c r="B397" s="91"/>
+      <c r="C397" s="91"/>
       <c r="D397" s="48" t="s">
         <v>1006</v>
       </c>
-      <c r="E397" s="100"/>
+      <c r="E397" s="93"/>
     </row>
     <row r="398" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A398" s="92">
+      <c r="A398" s="90">
         <v>5510313</v>
       </c>
-      <c r="B398" s="101" t="s">
+      <c r="B398" s="94" t="s">
         <v>1007</v>
       </c>
-      <c r="C398" s="92">
+      <c r="C398" s="90">
         <v>6510313</v>
       </c>
       <c r="D398" s="70" t="s">
         <v>1008</v>
       </c>
-      <c r="E398" s="99"/>
+      <c r="E398" s="92"/>
     </row>
     <row r="399" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A399" s="93"/>
-      <c r="B399" s="102"/>
-      <c r="C399" s="93"/>
+      <c r="A399" s="91"/>
+      <c r="B399" s="95"/>
+      <c r="C399" s="91"/>
       <c r="D399" s="48" t="s">
         <v>1009</v>
       </c>
-      <c r="E399" s="100"/>
+      <c r="E399" s="93"/>
     </row>
     <row r="400" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A400" s="47">
@@ -22572,28 +23207,28 @@
       <c r="E400" s="49"/>
     </row>
     <row r="401" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A401" s="92">
+      <c r="A401" s="90">
         <v>5510315</v>
       </c>
-      <c r="B401" s="101" t="s">
+      <c r="B401" s="94" t="s">
         <v>1011</v>
       </c>
-      <c r="C401" s="92">
+      <c r="C401" s="90">
         <v>6510315</v>
       </c>
       <c r="D401" s="70" t="s">
         <v>1012</v>
       </c>
-      <c r="E401" s="99"/>
+      <c r="E401" s="92"/>
     </row>
     <row r="402" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A402" s="93"/>
-      <c r="B402" s="102"/>
-      <c r="C402" s="93"/>
+      <c r="A402" s="91"/>
+      <c r="B402" s="95"/>
+      <c r="C402" s="91"/>
       <c r="D402" s="48" t="s">
         <v>1013</v>
       </c>
-      <c r="E402" s="100"/>
+      <c r="E402" s="93"/>
     </row>
     <row r="403" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A403" s="40">
@@ -25356,28 +25991,28 @@
       <c r="E602" s="49"/>
     </row>
     <row r="603" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A603" s="92">
+      <c r="A603" s="90">
         <v>5520147</v>
       </c>
-      <c r="B603" s="92" t="s">
+      <c r="B603" s="90" t="s">
         <v>1205</v>
       </c>
-      <c r="C603" s="92">
+      <c r="C603" s="90">
         <v>6520147</v>
       </c>
       <c r="D603" s="69" t="s">
         <v>1206</v>
       </c>
-      <c r="E603" s="99"/>
+      <c r="E603" s="92"/>
     </row>
     <row r="604" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A604" s="93"/>
-      <c r="B604" s="93"/>
-      <c r="C604" s="93"/>
+      <c r="A604" s="91"/>
+      <c r="B604" s="91"/>
+      <c r="C604" s="91"/>
       <c r="D604" s="48" t="s">
         <v>1207</v>
       </c>
-      <c r="E604" s="100"/>
+      <c r="E604" s="93"/>
     </row>
     <row r="605" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A605" s="47">
@@ -25454,28 +26089,28 @@
       <c r="E610" s="49"/>
     </row>
     <row r="611" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A611" s="92">
+      <c r="A611" s="90">
         <v>5520154</v>
       </c>
-      <c r="B611" s="101" t="s">
+      <c r="B611" s="94" t="s">
         <v>1214</v>
       </c>
-      <c r="C611" s="92">
+      <c r="C611" s="90">
         <v>6520154</v>
       </c>
       <c r="D611" s="69" t="s">
         <v>1215</v>
       </c>
-      <c r="E611" s="99"/>
+      <c r="E611" s="92"/>
     </row>
     <row r="612" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A612" s="93"/>
-      <c r="B612" s="102"/>
-      <c r="C612" s="93"/>
+      <c r="A612" s="91"/>
+      <c r="B612" s="95"/>
+      <c r="C612" s="91"/>
       <c r="D612" s="48" t="s">
         <v>1216</v>
       </c>
-      <c r="E612" s="100"/>
+      <c r="E612" s="93"/>
     </row>
     <row r="613" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A613" s="47">
@@ -25857,25 +26492,25 @@
       <c r="E645" s="49"/>
     </row>
     <row r="646" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A646" s="92">
+      <c r="A646" s="90">
         <v>5520184</v>
       </c>
-      <c r="B646" s="92" t="s">
+      <c r="B646" s="90" t="s">
         <v>1246</v>
       </c>
-      <c r="C646" s="92">
+      <c r="C646" s="90">
         <v>6520184</v>
       </c>
-      <c r="D646" s="92" t="s">
+      <c r="D646" s="90" t="s">
         <v>1246</v>
       </c>
       <c r="E646" s="66"/>
     </row>
     <row r="647" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A647" s="93"/>
-      <c r="B647" s="93"/>
-      <c r="C647" s="93"/>
-      <c r="D647" s="93"/>
+      <c r="A647" s="91"/>
+      <c r="B647" s="91"/>
+      <c r="C647" s="91"/>
+      <c r="D647" s="91"/>
       <c r="E647" s="49"/>
     </row>
     <row r="648" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -26727,35 +27362,35 @@
       <c r="E709" s="49"/>
     </row>
     <row r="710" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A710" s="92">
+      <c r="A710" s="90">
         <v>5520243</v>
       </c>
-      <c r="B710" s="92" t="s">
+      <c r="B710" s="90" t="s">
         <v>1307</v>
       </c>
-      <c r="C710" s="92">
+      <c r="C710" s="90">
         <v>6520243</v>
       </c>
-      <c r="D710" s="92" t="s">
+      <c r="D710" s="90" t="s">
         <v>1307</v>
       </c>
       <c r="E710" s="66"/>
     </row>
     <row r="711" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A711" s="93"/>
-      <c r="B711" s="93"/>
-      <c r="C711" s="93"/>
-      <c r="D711" s="93"/>
+      <c r="A711" s="91"/>
+      <c r="B711" s="91"/>
+      <c r="C711" s="91"/>
+      <c r="D711" s="91"/>
       <c r="E711" s="49"/>
     </row>
     <row r="712" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A712" s="92">
+      <c r="A712" s="90">
         <v>5520244</v>
       </c>
-      <c r="B712" s="92" t="s">
+      <c r="B712" s="90" t="s">
         <v>1308</v>
       </c>
-      <c r="C712" s="92">
+      <c r="C712" s="90">
         <v>6520244</v>
       </c>
       <c r="D712" s="69" t="s">
@@ -26773,9 +27408,9 @@
       <c r="E713" s="66"/>
     </row>
     <row r="714" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A714" s="93"/>
-      <c r="B714" s="93"/>
-      <c r="C714" s="93"/>
+      <c r="A714" s="91"/>
+      <c r="B714" s="91"/>
+      <c r="C714" s="91"/>
       <c r="D714" s="74"/>
       <c r="E714" s="49"/>
     </row>
@@ -26888,25 +27523,25 @@
       <c r="E722" s="49"/>
     </row>
     <row r="723" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A723" s="92">
+      <c r="A723" s="90">
         <v>5520251</v>
       </c>
-      <c r="B723" s="92" t="s">
+      <c r="B723" s="90" t="s">
         <v>1317</v>
       </c>
-      <c r="C723" s="92">
+      <c r="C723" s="90">
         <v>6520251</v>
       </c>
-      <c r="D723" s="92" t="s">
+      <c r="D723" s="90" t="s">
         <v>1317</v>
       </c>
       <c r="E723" s="66"/>
     </row>
     <row r="724" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A724" s="93"/>
-      <c r="B724" s="93"/>
-      <c r="C724" s="93"/>
-      <c r="D724" s="93"/>
+      <c r="A724" s="91"/>
+      <c r="B724" s="91"/>
+      <c r="C724" s="91"/>
+      <c r="D724" s="91"/>
       <c r="E724" s="49"/>
     </row>
     <row r="725" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -28083,25 +28718,25 @@
       <c r="E811" s="49"/>
     </row>
     <row r="812" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A812" s="94">
+      <c r="A812" s="99">
         <v>55402</v>
       </c>
-      <c r="B812" s="94" t="s">
+      <c r="B812" s="99" t="s">
         <v>1399</v>
       </c>
-      <c r="C812" s="94">
+      <c r="C812" s="99">
         <v>65402</v>
       </c>
-      <c r="D812" s="94" t="s">
+      <c r="D812" s="99" t="s">
         <v>1399</v>
       </c>
       <c r="E812" s="75"/>
     </row>
     <row r="813" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A813" s="95"/>
-      <c r="B813" s="95"/>
-      <c r="C813" s="95"/>
-      <c r="D813" s="95"/>
+      <c r="A813" s="100"/>
+      <c r="B813" s="100"/>
+      <c r="C813" s="100"/>
+      <c r="D813" s="100"/>
       <c r="E813" s="42"/>
     </row>
     <row r="814" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -28584,10 +29219,10 @@
       <c r="E850" s="49"/>
     </row>
     <row r="851" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A851" s="92">
+      <c r="A851" s="90">
         <v>5580209</v>
       </c>
-      <c r="B851" s="92" t="s">
+      <c r="B851" s="90" t="s">
         <v>1433</v>
       </c>
       <c r="C851" s="96"/>
@@ -28595,8 +29230,8 @@
       <c r="E851" s="66"/>
     </row>
     <row r="852" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A852" s="93"/>
-      <c r="B852" s="93"/>
+      <c r="A852" s="91"/>
+      <c r="B852" s="91"/>
       <c r="C852" s="97"/>
       <c r="D852" s="97"/>
       <c r="E852" s="49"/>
@@ -28999,25 +29634,25 @@
       <c r="E883" s="49"/>
     </row>
     <row r="884" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A884" s="92">
+      <c r="A884" s="90">
         <v>5620123</v>
       </c>
-      <c r="B884" s="92" t="s">
+      <c r="B884" s="90" t="s">
         <v>1462</v>
       </c>
-      <c r="C884" s="92">
+      <c r="C884" s="90">
         <v>6620123</v>
       </c>
-      <c r="D884" s="92" t="s">
+      <c r="D884" s="90" t="s">
         <v>1462</v>
       </c>
       <c r="E884" s="66"/>
     </row>
     <row r="885" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A885" s="93"/>
-      <c r="B885" s="93"/>
-      <c r="C885" s="93"/>
-      <c r="D885" s="93"/>
+      <c r="A885" s="91"/>
+      <c r="B885" s="91"/>
+      <c r="C885" s="91"/>
+      <c r="D885" s="91"/>
       <c r="E885" s="49"/>
     </row>
     <row r="886" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -31197,28 +31832,28 @@
       <c r="E1045" s="49"/>
     </row>
     <row r="1046" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1046" s="94">
+      <c r="A1046" s="99">
         <v>58402</v>
       </c>
-      <c r="B1046" s="94" t="s">
+      <c r="B1046" s="99" t="s">
         <v>1611</v>
       </c>
-      <c r="C1046" s="94">
+      <c r="C1046" s="99">
         <v>68402</v>
       </c>
       <c r="D1046" s="69" t="s">
         <v>1612</v>
       </c>
-      <c r="E1046" s="90"/>
+      <c r="E1046" s="101"/>
     </row>
     <row r="1047" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1047" s="95"/>
-      <c r="B1047" s="95"/>
-      <c r="C1047" s="95"/>
+      <c r="A1047" s="100"/>
+      <c r="B1047" s="100"/>
+      <c r="C1047" s="100"/>
       <c r="D1047" s="41" t="s">
         <v>1611</v>
       </c>
-      <c r="E1047" s="91"/>
+      <c r="E1047" s="102"/>
     </row>
     <row r="1048" spans="1:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1048" s="47">
@@ -32304,52 +32939,14 @@
     </row>
   </sheetData>
   <mergeCells count="69">
-    <mergeCell ref="A68:A69"/>
-    <mergeCell ref="B68:B69"/>
-    <mergeCell ref="C68:C69"/>
-    <mergeCell ref="D68:D69"/>
-    <mergeCell ref="A230:A231"/>
-    <mergeCell ref="C230:C231"/>
-    <mergeCell ref="E230:E231"/>
-    <mergeCell ref="A235:A236"/>
-    <mergeCell ref="C235:C236"/>
-    <mergeCell ref="E235:E236"/>
-    <mergeCell ref="A343:A344"/>
-    <mergeCell ref="B343:B344"/>
-    <mergeCell ref="C343:C344"/>
-    <mergeCell ref="E343:E344"/>
-    <mergeCell ref="A378:A379"/>
-    <mergeCell ref="B378:B379"/>
-    <mergeCell ref="C378:C379"/>
-    <mergeCell ref="E378:E379"/>
-    <mergeCell ref="A396:A397"/>
-    <mergeCell ref="B396:B397"/>
-    <mergeCell ref="C396:C397"/>
-    <mergeCell ref="E396:E397"/>
-    <mergeCell ref="A398:A399"/>
-    <mergeCell ref="B398:B399"/>
-    <mergeCell ref="C398:C399"/>
-    <mergeCell ref="E398:E399"/>
-    <mergeCell ref="A401:A402"/>
-    <mergeCell ref="B401:B402"/>
-    <mergeCell ref="C401:C402"/>
-    <mergeCell ref="E401:E402"/>
-    <mergeCell ref="A603:A604"/>
-    <mergeCell ref="B603:B604"/>
-    <mergeCell ref="C603:C604"/>
-    <mergeCell ref="E603:E604"/>
-    <mergeCell ref="A611:A612"/>
-    <mergeCell ref="B611:B612"/>
-    <mergeCell ref="C611:C612"/>
-    <mergeCell ref="E611:E612"/>
-    <mergeCell ref="A646:A647"/>
-    <mergeCell ref="B646:B647"/>
-    <mergeCell ref="C646:C647"/>
-    <mergeCell ref="D646:D647"/>
-    <mergeCell ref="A710:A711"/>
-    <mergeCell ref="B710:B711"/>
-    <mergeCell ref="C710:C711"/>
-    <mergeCell ref="D710:D711"/>
+    <mergeCell ref="E1046:E1047"/>
+    <mergeCell ref="A884:A885"/>
+    <mergeCell ref="B884:B885"/>
+    <mergeCell ref="C884:C885"/>
+    <mergeCell ref="D884:D885"/>
+    <mergeCell ref="A1046:A1047"/>
+    <mergeCell ref="B1046:B1047"/>
+    <mergeCell ref="C1046:C1047"/>
     <mergeCell ref="A851:A852"/>
     <mergeCell ref="B851:B852"/>
     <mergeCell ref="C851:C852"/>
@@ -32365,40 +32962,84 @@
     <mergeCell ref="B812:B813"/>
     <mergeCell ref="C812:C813"/>
     <mergeCell ref="D812:D813"/>
-    <mergeCell ref="E1046:E1047"/>
-    <mergeCell ref="A884:A885"/>
-    <mergeCell ref="B884:B885"/>
-    <mergeCell ref="C884:C885"/>
-    <mergeCell ref="D884:D885"/>
-    <mergeCell ref="A1046:A1047"/>
-    <mergeCell ref="B1046:B1047"/>
-    <mergeCell ref="C1046:C1047"/>
+    <mergeCell ref="A646:A647"/>
+    <mergeCell ref="B646:B647"/>
+    <mergeCell ref="C646:C647"/>
+    <mergeCell ref="D646:D647"/>
+    <mergeCell ref="A710:A711"/>
+    <mergeCell ref="B710:B711"/>
+    <mergeCell ref="C710:C711"/>
+    <mergeCell ref="D710:D711"/>
+    <mergeCell ref="A603:A604"/>
+    <mergeCell ref="B603:B604"/>
+    <mergeCell ref="C603:C604"/>
+    <mergeCell ref="E603:E604"/>
+    <mergeCell ref="A611:A612"/>
+    <mergeCell ref="B611:B612"/>
+    <mergeCell ref="C611:C612"/>
+    <mergeCell ref="E611:E612"/>
+    <mergeCell ref="A398:A399"/>
+    <mergeCell ref="B398:B399"/>
+    <mergeCell ref="C398:C399"/>
+    <mergeCell ref="E398:E399"/>
+    <mergeCell ref="A401:A402"/>
+    <mergeCell ref="B401:B402"/>
+    <mergeCell ref="C401:C402"/>
+    <mergeCell ref="E401:E402"/>
+    <mergeCell ref="A378:A379"/>
+    <mergeCell ref="B378:B379"/>
+    <mergeCell ref="C378:C379"/>
+    <mergeCell ref="E378:E379"/>
+    <mergeCell ref="A396:A397"/>
+    <mergeCell ref="B396:B397"/>
+    <mergeCell ref="C396:C397"/>
+    <mergeCell ref="E396:E397"/>
+    <mergeCell ref="E230:E231"/>
+    <mergeCell ref="A235:A236"/>
+    <mergeCell ref="C235:C236"/>
+    <mergeCell ref="E235:E236"/>
+    <mergeCell ref="A343:A344"/>
+    <mergeCell ref="B343:B344"/>
+    <mergeCell ref="C343:C344"/>
+    <mergeCell ref="E343:E344"/>
+    <mergeCell ref="A68:A69"/>
+    <mergeCell ref="B68:B69"/>
+    <mergeCell ref="C68:C69"/>
+    <mergeCell ref="D68:D69"/>
+    <mergeCell ref="A230:A231"/>
+    <mergeCell ref="C230:C231"/>
   </mergeCells>
   <conditionalFormatting sqref="G4:H9">
-    <cfRule type="duplicateValues" dxfId="7" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I1:BM1">
-    <cfRule type="notContainsBlanks" dxfId="6" priority="7">
+  <conditionalFormatting sqref="I1:BQ1">
+    <cfRule type="notContainsBlanks" dxfId="19" priority="9">
       <formula>LEN(TRIM(I1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I3:BM3">
-    <cfRule type="duplicateValues" dxfId="5" priority="3"/>
+  <conditionalFormatting sqref="I4:BQ4">
+    <cfRule type="duplicateValues" dxfId="18" priority="6"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I4:BM4">
-    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
+  <conditionalFormatting sqref="I5:BO5 BQ4">
+    <cfRule type="duplicateValues" dxfId="17" priority="7"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I5:BM5">
-    <cfRule type="duplicateValues" dxfId="3" priority="5"/>
+  <conditionalFormatting sqref="I6:BO6 BQ5">
+    <cfRule type="duplicateValues" dxfId="16" priority="8"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I6:BM6">
-    <cfRule type="duplicateValues" dxfId="2" priority="6"/>
+  <conditionalFormatting sqref="I7:BO7 BQ6">
+    <cfRule type="duplicateValues" dxfId="15" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I7:BM7">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  <conditionalFormatting sqref="I8:BO8 BQ7">
+    <cfRule type="duplicateValues" dxfId="14" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I8:BM8">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  <conditionalFormatting sqref="I3:BO3">
+    <cfRule type="duplicateValues" dxfId="13" priority="11"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BP3:BP32">
+    <cfRule type="duplicateValues" dxfId="12" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BQ3">
+    <cfRule type="duplicateValues" dxfId="11" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>